<commit_message>
agrego crosswalks argentina y mesico
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Guido\Trabajo\Economia\Tematicas de Investigacion\Precariedad Mundial\precariedad.mundial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96402554-77CE-4454-8768-E476EB8D15A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A8133B-8C51-4481-89B1-F65EFB93BAF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miwbJz/ooLDg0TpP5RJ4gNcrXXX9A=="/>
     </ext>
   </extLst>
 </workbook>
@@ -78,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5819" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5842" uniqueCount="1081">
   <si>
     <t>Pais</t>
   </si>
@@ -3209,9 +3206,6 @@
     <t>¿Cuál fue el sueldo o salario mensual sin descuentos que (………) recibió en este trabajo? (ocupación principal)</t>
   </si>
   <si>
-    <t>Periodicidad</t>
-  </si>
-  <si>
     <t>Trimestral</t>
   </si>
   <si>
@@ -3305,17 +3299,69 @@
   </si>
   <si>
     <t xml:space="preserve">2002 - 2020: Encuestas en meses puntuales del año. 2019 en Mayo y Noviembre </t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Usar 1er trimestre</t>
+  </si>
+  <si>
+    <t>Usar única base</t>
+  </si>
+  <si>
+    <t>Promediar</t>
+  </si>
+  <si>
+    <t>Usar base Marzo</t>
+  </si>
+  <si>
+    <t>Periodicidad bases</t>
+  </si>
+  <si>
+    <t>Argenina</t>
+  </si>
+  <si>
+    <t>PP04D_COD</t>
+  </si>
+  <si>
+    <t>CON 2001</t>
+  </si>
+  <si>
+    <t>Encontre crosswalk</t>
+  </si>
+  <si>
+    <t>GRUPOS CIUO</t>
+  </si>
+  <si>
+    <t>4 niveles de calificación asimilables a los de CIUO y EPH</t>
+  </si>
+  <si>
+    <t>Cruce ad-hoc</t>
+  </si>
+  <si>
+    <t>En curso cross c tablas oficiales</t>
+  </si>
+  <si>
+    <t>Chequeo 17-5-2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3727,281 +3773,282 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="4"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="4"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo 2" xfId="2" xr:uid="{4F722B9A-536A-46D8-AFD0-3E32E4A5CDA5}"/>
@@ -5022,215 +5069,215 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="83" t="s">
+      <c r="C31" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D31" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="83">
+      <c r="E31" s="82">
         <v>1</v>
       </c>
-      <c r="F31" s="82" t="s">
+      <c r="F31" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="82" t="s">
+      <c r="G31" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H31" s="82" t="s">
+      <c r="H31" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="J31" s="69"/>
+      <c r="J31" s="68"/>
     </row>
     <row r="32" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="82" t="s">
+      <c r="B32" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="82" t="s">
+      <c r="D32" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="83">
+      <c r="E32" s="82">
         <v>2</v>
       </c>
-      <c r="F32" s="82" t="s">
+      <c r="F32" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="82" t="s">
+      <c r="G32" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H32" s="82" t="s">
+      <c r="H32" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="69"/>
-    </row>
-    <row r="33" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A33" s="82" t="s">
+      <c r="J32" s="68"/>
+    </row>
+    <row r="33" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A33" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="82" t="s">
+      <c r="B33" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="83" t="s">
+      <c r="C33" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="83">
+      <c r="E33" s="82">
         <v>3</v>
       </c>
-      <c r="F33" s="82" t="s">
+      <c r="F33" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="82" t="s">
+      <c r="G33" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H33" s="82" t="s">
+      <c r="H33" s="81" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A34" s="82" t="s">
+    <row r="34" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A34" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="82" t="s">
+      <c r="B34" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="84" t="s">
+      <c r="C34" s="83" t="s">
         <v>946</v>
       </c>
-      <c r="D34" s="85" t="s">
+      <c r="D34" s="84" t="s">
         <v>947</v>
       </c>
-      <c r="E34" s="83">
+      <c r="E34" s="82">
         <v>1</v>
       </c>
-      <c r="F34" s="82" t="s">
+      <c r="F34" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G34" s="82" t="s">
+      <c r="G34" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H34" s="82" t="s">
+      <c r="H34" s="81" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A35" s="82" t="s">
+    <row r="35" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A35" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="82" t="s">
+      <c r="B35" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="83" t="s">
         <v>946</v>
       </c>
-      <c r="D35" s="85" t="s">
+      <c r="D35" s="84" t="s">
         <v>947</v>
       </c>
-      <c r="E35" s="83">
+      <c r="E35" s="82">
         <v>2</v>
       </c>
-      <c r="F35" s="82" t="s">
+      <c r="F35" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G35" s="82" t="s">
+      <c r="G35" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="82" t="s">
+      <c r="H35" s="81" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A36" s="82" t="s">
+    <row r="36" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A36" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="82" t="s">
+      <c r="B36" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="84" t="s">
+      <c r="C36" s="83" t="s">
         <v>946</v>
       </c>
-      <c r="D36" s="85" t="s">
+      <c r="D36" s="84" t="s">
         <v>947</v>
       </c>
-      <c r="E36" s="83">
+      <c r="E36" s="82">
         <v>9</v>
       </c>
-      <c r="F36" s="82" t="s">
+      <c r="F36" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="G36" s="82" t="s">
+      <c r="G36" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H36" s="82" t="s">
+      <c r="H36" s="81" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A37" s="82" t="s">
+    <row r="37" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A37" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="84" t="s">
+      <c r="C37" s="83" t="s">
         <v>940</v>
       </c>
-      <c r="D37" s="85" t="s">
+      <c r="D37" s="84" t="s">
         <v>941</v>
       </c>
-      <c r="E37" s="83">
+      <c r="E37" s="82">
         <v>4</v>
       </c>
-      <c r="F37" s="82" t="s">
+      <c r="F37" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G37" s="82" t="s">
+      <c r="G37" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H37" s="82" t="s">
+      <c r="H37" s="81" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="84" t="s">
+      <c r="C38" s="83" t="s">
         <v>940</v>
       </c>
-      <c r="D38" s="85" t="s">
+      <c r="D38" s="84" t="s">
         <v>941</v>
       </c>
-      <c r="E38" s="83" t="s">
+      <c r="E38" s="82" t="s">
         <v>731</v>
       </c>
-      <c r="F38" s="82" t="s">
+      <c r="F38" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G38" s="82" t="s">
+      <c r="G38" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H38" s="82" t="s">
+      <c r="H38" s="81" t="s">
         <v>945</v>
       </c>
-      <c r="J38" s="69"/>
+      <c r="J38" s="68"/>
     </row>
     <row r="39" spans="1:10" ht="14.3" customHeight="1">
       <c r="A39" s="4" t="s">
@@ -5684,11 +5731,11 @@
       <c r="C56" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="122" t="s">
+      <c r="D56" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="E56" s="123"/>
-      <c r="F56" s="123"/>
+      <c r="E56" s="125"/>
+      <c r="F56" s="125"/>
       <c r="G56" s="4" t="s">
         <v>27</v>
       </c>
@@ -5706,11 +5753,11 @@
       <c r="C57" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="122" t="s">
+      <c r="D57" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="E57" s="123"/>
-      <c r="F57" s="123"/>
+      <c r="E57" s="125"/>
+      <c r="F57" s="125"/>
       <c r="G57" s="4" t="s">
         <v>27</v>
       </c>
@@ -5728,11 +5775,11 @@
       <c r="C58" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="122" t="s">
+      <c r="D58" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="E58" s="123"/>
-      <c r="F58" s="123"/>
+      <c r="E58" s="125"/>
+      <c r="F58" s="125"/>
       <c r="G58" s="4" t="s">
         <v>27</v>
       </c>
@@ -5750,11 +5797,11 @@
       <c r="C59" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="122" t="s">
+      <c r="D59" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="E59" s="123"/>
-      <c r="F59" s="123"/>
+      <c r="E59" s="125"/>
+      <c r="F59" s="125"/>
       <c r="G59" s="4" t="s">
         <v>27</v>
       </c>
@@ -6491,342 +6538,342 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A88" s="82" t="s">
+      <c r="A88" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B88" s="82" t="s">
+      <c r="B88" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C88" s="83" t="s">
+      <c r="C88" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="D88" s="82" t="s">
+      <c r="D88" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="E88" s="83">
+      <c r="E88" s="82">
         <v>1</v>
       </c>
-      <c r="F88" s="82" t="s">
+      <c r="F88" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G88" s="82" t="s">
+      <c r="G88" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H88" s="82" t="s">
+      <c r="H88" s="81" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A89" s="82" t="s">
+      <c r="A89" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="82" t="s">
+      <c r="B89" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C89" s="83" t="s">
+      <c r="C89" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="D89" s="82" t="s">
+      <c r="D89" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="E89" s="83">
+      <c r="E89" s="82">
         <v>2</v>
       </c>
-      <c r="F89" s="82" t="s">
+      <c r="F89" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G89" s="82" t="s">
+      <c r="G89" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H89" s="82" t="s">
+      <c r="H89" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A90" s="82" t="s">
+      <c r="A90" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="82" t="s">
+      <c r="B90" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C90" s="83" t="s">
+      <c r="C90" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="D90" s="82" t="s">
+      <c r="D90" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="E90" s="83">
+      <c r="E90" s="82">
         <v>1</v>
       </c>
-      <c r="F90" s="82" t="s">
+      <c r="F90" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="G90" s="82" t="s">
+      <c r="G90" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H90" s="82" t="s">
+      <c r="H90" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A91" s="82" t="s">
+      <c r="A91" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B91" s="82" t="s">
+      <c r="B91" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="83" t="s">
+      <c r="C91" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="D91" s="82" t="s">
+      <c r="D91" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="E91" s="83">
+      <c r="E91" s="82">
         <v>2</v>
       </c>
-      <c r="F91" s="82" t="s">
+      <c r="F91" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="G91" s="82" t="s">
+      <c r="G91" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H91" s="82" t="s">
+      <c r="H91" s="81" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A92" s="82" t="s">
+      <c r="A92" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B92" s="82" t="s">
+      <c r="B92" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C92" s="83" t="s">
+      <c r="C92" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="D92" s="82" t="s">
+      <c r="D92" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="E92" s="83">
+      <c r="E92" s="82">
         <v>3</v>
       </c>
-      <c r="F92" s="82" t="s">
+      <c r="F92" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="G92" s="82" t="s">
+      <c r="G92" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H92" s="82" t="s">
+      <c r="H92" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A93" s="82" t="s">
+      <c r="A93" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B93" s="82" t="s">
+      <c r="B93" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C93" s="82" t="s">
+      <c r="C93" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="D93" s="82" t="s">
+      <c r="D93" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="E93" s="83">
+      <c r="E93" s="82">
         <v>1</v>
       </c>
-      <c r="F93" s="82" t="s">
+      <c r="F93" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G93" s="82" t="s">
+      <c r="G93" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H93" s="82" t="s">
+      <c r="H93" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A94" s="82" t="s">
+      <c r="A94" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B94" s="82" t="s">
+      <c r="B94" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C94" s="82" t="s">
+      <c r="C94" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="D94" s="82" t="s">
+      <c r="D94" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="E94" s="83">
+      <c r="E94" s="82">
         <v>2</v>
       </c>
-      <c r="F94" s="82" t="s">
+      <c r="F94" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G94" s="82" t="s">
+      <c r="G94" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H94" s="82" t="s">
+      <c r="H94" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A95" s="82" t="s">
+      <c r="A95" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B95" s="82" t="s">
+      <c r="B95" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C95" s="82" t="s">
+      <c r="C95" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="D95" s="82" t="s">
+      <c r="D95" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="E95" s="83">
+      <c r="E95" s="82">
         <v>1</v>
       </c>
-      <c r="F95" s="82" t="s">
+      <c r="F95" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G95" s="82" t="s">
+      <c r="G95" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H95" s="82" t="s">
+      <c r="H95" s="81" t="s">
         <v>944</v>
       </c>
-      <c r="J95" s="69"/>
+      <c r="J95" s="68"/>
     </row>
     <row r="96" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A96" s="82" t="s">
+      <c r="A96" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B96" s="82" t="s">
+      <c r="B96" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C96" s="82" t="s">
+      <c r="C96" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="D96" s="82" t="s">
+      <c r="D96" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="E96" s="83">
+      <c r="E96" s="82">
         <v>2</v>
       </c>
-      <c r="F96" s="82" t="s">
+      <c r="F96" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G96" s="82" t="s">
+      <c r="G96" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H96" s="82" t="s">
+      <c r="H96" s="81" t="s">
         <v>945</v>
       </c>
-      <c r="J96" s="69"/>
+      <c r="J96" s="68"/>
     </row>
     <row r="97" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A97" s="82" t="s">
+      <c r="A97" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B97" s="82" t="s">
+      <c r="B97" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C97" s="82" t="s">
+      <c r="C97" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="D97" s="82" t="s">
+      <c r="D97" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="E97" s="83">
+      <c r="E97" s="82">
         <v>1</v>
       </c>
-      <c r="F97" s="86" t="s">
+      <c r="F97" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="G97" s="82" t="s">
+      <c r="G97" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H97" s="82" t="s">
+      <c r="H97" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A98" s="82" t="s">
+      <c r="A98" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B98" s="82" t="s">
+      <c r="B98" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C98" s="82" t="s">
+      <c r="C98" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="D98" s="82" t="s">
+      <c r="D98" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="E98" s="83">
+      <c r="E98" s="82">
         <v>2</v>
       </c>
-      <c r="F98" s="86" t="s">
+      <c r="F98" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="G98" s="82" t="s">
+      <c r="G98" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H98" s="82" t="s">
+      <c r="H98" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A99" s="82" t="s">
+      <c r="A99" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B99" s="82" t="s">
+      <c r="B99" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C99" s="82" t="s">
+      <c r="C99" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="D99" s="82" t="s">
+      <c r="D99" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="E99" s="83">
+      <c r="E99" s="82">
         <v>3</v>
       </c>
-      <c r="F99" s="86" t="s">
+      <c r="F99" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="G99" s="82" t="s">
+      <c r="G99" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H99" s="82" t="s">
+      <c r="H99" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A100" s="82" t="s">
+      <c r="A100" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="B100" s="82" t="s">
+      <c r="B100" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C100" s="82" t="s">
+      <c r="C100" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="D100" s="82" t="s">
+      <c r="D100" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="E100" s="83">
+      <c r="E100" s="82">
         <v>4</v>
       </c>
-      <c r="F100" s="86" t="s">
+      <c r="F100" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="G100" s="82" t="s">
+      <c r="G100" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H100" s="82" t="s">
+      <c r="H100" s="81" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8255,164 +8302,164 @@
       </c>
     </row>
     <row r="158" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A158" s="82" t="s">
+      <c r="A158" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B158" s="82" t="s">
+      <c r="B158" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C158" s="83" t="s">
+      <c r="C158" s="82" t="s">
         <v>229</v>
       </c>
-      <c r="D158" s="82" t="s">
+      <c r="D158" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="E158" s="83">
+      <c r="E158" s="82">
         <v>1</v>
       </c>
-      <c r="F158" s="82" t="s">
+      <c r="F158" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G158" s="82" t="s">
+      <c r="G158" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H158" s="82" t="s">
+      <c r="H158" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="J158" s="69"/>
+      <c r="J158" s="68"/>
     </row>
     <row r="159" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A159" s="82" t="s">
+      <c r="A159" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B159" s="82" t="s">
+      <c r="B159" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C159" s="83" t="s">
+      <c r="C159" s="82" t="s">
         <v>229</v>
       </c>
-      <c r="D159" s="82" t="s">
+      <c r="D159" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="E159" s="83">
+      <c r="E159" s="82">
         <v>2</v>
       </c>
-      <c r="F159" s="82" t="s">
+      <c r="F159" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G159" s="82" t="s">
+      <c r="G159" s="81" t="s">
         <v>948</v>
       </c>
-      <c r="H159" s="82" t="s">
+      <c r="H159" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="J159" s="69"/>
-    </row>
-    <row r="160" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A160" s="82" t="s">
+      <c r="J159" s="68"/>
+    </row>
+    <row r="160" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A160" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B160" s="82" t="s">
+      <c r="B160" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C160" s="83" t="s">
+      <c r="C160" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D160" s="82" t="s">
+      <c r="D160" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="E160" s="83">
+      <c r="E160" s="82">
         <v>1</v>
       </c>
-      <c r="F160" s="82" t="s">
+      <c r="F160" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G160" s="82" t="s">
+      <c r="G160" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H160" s="82" t="s">
+      <c r="H160" s="81" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="161" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A161" s="82" t="s">
+    <row r="161" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A161" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B161" s="82" t="s">
+      <c r="B161" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C161" s="83" t="s">
+      <c r="C161" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D161" s="82" t="s">
+      <c r="D161" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="E161" s="83">
+      <c r="E161" s="82">
         <v>2</v>
       </c>
-      <c r="F161" s="82" t="s">
+      <c r="F161" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G161" s="82" t="s">
+      <c r="G161" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H161" s="82" t="s">
+      <c r="H161" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A162" s="82" t="s">
+      <c r="A162" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B162" s="82" t="s">
+      <c r="B162" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C162" s="83" t="s">
+      <c r="C162" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D162" s="82" t="s">
+      <c r="D162" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="E162" s="83">
+      <c r="E162" s="82">
         <v>1</v>
       </c>
-      <c r="F162" s="82" t="s">
+      <c r="F162" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G162" s="82" t="s">
+      <c r="G162" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H162" s="82" t="s">
+      <c r="H162" s="81" t="s">
         <v>944</v>
       </c>
-      <c r="J162" s="69"/>
+      <c r="J162" s="68"/>
     </row>
     <row r="163" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A163" s="82" t="s">
+      <c r="A163" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="B163" s="82" t="s">
+      <c r="B163" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C163" s="83" t="s">
+      <c r="C163" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D163" s="82" t="s">
+      <c r="D163" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="E163" s="83">
+      <c r="E163" s="82">
         <v>2</v>
       </c>
-      <c r="F163" s="82" t="s">
+      <c r="F163" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G163" s="82" t="s">
+      <c r="G163" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H163" s="82" t="s">
+      <c r="H163" s="81" t="s">
         <v>945</v>
       </c>
-      <c r="J163" s="69"/>
+      <c r="J163" s="68"/>
     </row>
     <row r="164" spans="1:10" ht="14.3" customHeight="1">
       <c r="A164" s="4" t="s">
@@ -9540,159 +9587,159 @@
         <v>228</v>
       </c>
     </row>
-    <row r="208" spans="1:8" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A208" s="82" t="s">
+    <row r="208" spans="1:8" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A208" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B208" s="82" t="s">
+      <c r="B208" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C208" s="82" t="s">
+      <c r="C208" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="D208" s="82" t="s">
+      <c r="D208" s="81" t="s">
         <v>949</v>
       </c>
       <c r="E208" s="54" t="s">
         <v>950</v>
       </c>
-      <c r="F208" s="68" t="s">
+      <c r="F208" s="67" t="s">
         <v>308</v>
       </c>
-      <c r="G208" s="82" t="s">
+      <c r="G208" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H208" s="68" t="s">
+      <c r="H208" s="67" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A209" s="82" t="s">
+    <row r="209" spans="1:8" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A209" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B209" s="82" t="s">
+      <c r="B209" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C209" s="82" t="s">
+      <c r="C209" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="D209" s="82" t="s">
+      <c r="D209" s="81" t="s">
         <v>949</v>
       </c>
       <c r="E209" s="54" t="s">
         <v>951</v>
       </c>
-      <c r="F209" s="68" t="s">
+      <c r="F209" s="67" t="s">
         <v>309</v>
       </c>
-      <c r="G209" s="82" t="s">
+      <c r="G209" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H209" s="68" t="s">
+      <c r="H209" s="67" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A210" s="82" t="s">
+    <row r="210" spans="1:8" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A210" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B210" s="82" t="s">
+      <c r="B210" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C210" s="82" t="s">
+      <c r="C210" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="D210" s="82" t="s">
+      <c r="D210" s="81" t="s">
         <v>949</v>
       </c>
       <c r="E210" s="54" t="s">
         <v>952</v>
       </c>
-      <c r="F210" s="68" t="s">
+      <c r="F210" s="67" t="s">
         <v>310</v>
       </c>
-      <c r="G210" s="82" t="s">
+      <c r="G210" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H210" s="68" t="s">
+      <c r="H210" s="67" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A211" s="82" t="s">
+    <row r="211" spans="1:8" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A211" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B211" s="82" t="s">
+      <c r="B211" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C211" s="82" t="s">
+      <c r="C211" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="D211" s="82" t="s">
+      <c r="D211" s="81" t="s">
         <v>949</v>
       </c>
       <c r="E211" s="54" t="s">
         <v>953</v>
       </c>
-      <c r="F211" s="68" t="s">
+      <c r="F211" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="G211" s="82" t="s">
+      <c r="G211" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H211" s="68" t="s">
+      <c r="H211" s="67" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A212" s="82" t="s">
+      <c r="A212" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B212" s="82" t="s">
+      <c r="B212" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C212" s="82" t="s">
+      <c r="C212" s="81" t="s">
         <v>284</v>
       </c>
-      <c r="D212" s="82" t="s">
+      <c r="D212" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="E212" s="83">
+      <c r="E212" s="82">
         <v>1</v>
       </c>
-      <c r="F212" s="82" t="s">
+      <c r="F212" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="G212" s="82" t="s">
+      <c r="G212" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H212" s="82" t="s">
+      <c r="H212" s="81" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="213" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A213" s="82" t="s">
+      <c r="A213" s="81" t="s">
         <v>257</v>
       </c>
-      <c r="B213" s="82" t="s">
+      <c r="B213" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="C213" s="82" t="s">
+      <c r="C213" s="81" t="s">
         <v>284</v>
       </c>
-      <c r="D213" s="82" t="s">
+      <c r="D213" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="E213" s="83">
+      <c r="E213" s="82">
         <v>2</v>
       </c>
-      <c r="F213" s="82" t="s">
+      <c r="F213" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="G213" s="82" t="s">
+      <c r="G213" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H213" s="82" t="s">
+      <c r="H213" s="81" t="s">
         <v>30</v>
       </c>
     </row>
@@ -11082,299 +11129,299 @@
         <v>228</v>
       </c>
     </row>
-    <row r="268" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A268" s="82" t="s">
+    <row r="268" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A268" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B268" s="82" t="s">
+      <c r="B268" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C268" s="69" t="s">
+      <c r="C268" s="68" t="s">
         <v>355</v>
       </c>
-      <c r="D268" s="91" t="s">
+      <c r="D268" s="90" t="s">
         <v>956</v>
       </c>
       <c r="E268" s="54">
         <v>1</v>
       </c>
-      <c r="F268" s="68" t="s">
+      <c r="F268" s="67" t="s">
         <v>954</v>
       </c>
-      <c r="G268" s="82" t="s">
+      <c r="G268" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H268" s="68" t="s">
+      <c r="H268" s="67" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="269" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A269" s="82" t="s">
+    <row r="269" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A269" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B269" s="82" t="s">
+      <c r="B269" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C269" s="69" t="s">
+      <c r="C269" s="68" t="s">
         <v>355</v>
       </c>
-      <c r="D269" s="91" t="s">
+      <c r="D269" s="90" t="s">
         <v>956</v>
       </c>
       <c r="E269" s="54">
         <v>2</v>
       </c>
-      <c r="F269" s="68" t="s">
+      <c r="F269" s="67" t="s">
         <v>955</v>
       </c>
-      <c r="G269" s="82" t="s">
+      <c r="G269" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H269" s="68" t="s">
+      <c r="H269" s="67" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="270" spans="1:10" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A270" s="82" t="s">
+    <row r="270" spans="1:10" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A270" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B270" s="82" t="s">
+      <c r="B270" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C270" s="69" t="s">
+      <c r="C270" s="68" t="s">
         <v>355</v>
       </c>
-      <c r="D270" s="91" t="s">
+      <c r="D270" s="90" t="s">
         <v>956</v>
       </c>
       <c r="E270" s="54">
         <v>3</v>
       </c>
-      <c r="F270" s="68" t="s">
+      <c r="F270" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="G270" s="82" t="s">
+      <c r="G270" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H270" s="68" t="s">
+      <c r="H270" s="67" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="271" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A271" s="82" t="s">
+      <c r="A271" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B271" s="82" t="s">
+      <c r="B271" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C271" s="82" t="s">
+      <c r="C271" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D271" s="82" t="s">
+      <c r="D271" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E271" s="89">
+      <c r="E271" s="88">
         <v>1</v>
       </c>
-      <c r="F271" s="90" t="s">
+      <c r="F271" s="89" t="s">
         <v>347</v>
       </c>
-      <c r="G271" s="82" t="s">
+      <c r="G271" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H271" s="82" t="s">
+      <c r="H271" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J271" s="69"/>
+      <c r="J271" s="68"/>
     </row>
     <row r="272" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A272" s="82" t="s">
+      <c r="A272" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B272" s="82" t="s">
+      <c r="B272" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C272" s="82" t="s">
+      <c r="C272" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D272" s="82" t="s">
+      <c r="D272" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E272" s="89">
+      <c r="E272" s="88">
         <v>2</v>
       </c>
-      <c r="F272" s="90" t="s">
+      <c r="F272" s="89" t="s">
         <v>348</v>
       </c>
-      <c r="G272" s="82" t="s">
+      <c r="G272" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H272" s="82" t="s">
+      <c r="H272" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J272" s="69"/>
+      <c r="J272" s="68"/>
     </row>
     <row r="273" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A273" s="82" t="s">
+      <c r="A273" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B273" s="82" t="s">
+      <c r="B273" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C273" s="82" t="s">
+      <c r="C273" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D273" s="82" t="s">
+      <c r="D273" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E273" s="89">
+      <c r="E273" s="88">
         <v>3</v>
       </c>
-      <c r="F273" s="90" t="s">
+      <c r="F273" s="89" t="s">
         <v>349</v>
       </c>
-      <c r="G273" s="82" t="s">
+      <c r="G273" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H273" s="82" t="s">
+      <c r="H273" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J273" s="69"/>
+      <c r="J273" s="68"/>
     </row>
     <row r="274" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A274" s="82" t="s">
+      <c r="A274" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B274" s="82" t="s">
+      <c r="B274" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C274" s="82" t="s">
+      <c r="C274" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D274" s="82" t="s">
+      <c r="D274" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E274" s="89">
+      <c r="E274" s="88">
         <v>4</v>
       </c>
-      <c r="F274" s="90" t="s">
+      <c r="F274" s="89" t="s">
         <v>350</v>
       </c>
-      <c r="G274" s="82" t="s">
+      <c r="G274" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H274" s="82" t="s">
+      <c r="H274" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J274" s="69"/>
+      <c r="J274" s="68"/>
     </row>
     <row r="275" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A275" s="82" t="s">
+      <c r="A275" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B275" s="82" t="s">
+      <c r="B275" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C275" s="82" t="s">
+      <c r="C275" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D275" s="82" t="s">
+      <c r="D275" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E275" s="89">
+      <c r="E275" s="88">
         <v>5</v>
       </c>
-      <c r="F275" s="90" t="s">
+      <c r="F275" s="89" t="s">
         <v>351</v>
       </c>
-      <c r="G275" s="82" t="s">
+      <c r="G275" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H275" s="82" t="s">
+      <c r="H275" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J275" s="69"/>
+      <c r="J275" s="68"/>
     </row>
     <row r="276" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A276" s="82" t="s">
+      <c r="A276" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B276" s="82" t="s">
+      <c r="B276" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C276" s="82" t="s">
+      <c r="C276" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D276" s="82" t="s">
+      <c r="D276" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E276" s="89">
+      <c r="E276" s="88">
         <v>6</v>
       </c>
-      <c r="F276" s="90" t="s">
+      <c r="F276" s="89" t="s">
         <v>352</v>
       </c>
-      <c r="G276" s="82" t="s">
+      <c r="G276" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H276" s="82" t="s">
+      <c r="H276" s="81" t="s">
         <v>942</v>
       </c>
-      <c r="J276" s="69"/>
+      <c r="J276" s="68"/>
     </row>
     <row r="277" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A277" s="82" t="s">
+      <c r="A277" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B277" s="82" t="s">
+      <c r="B277" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C277" s="82" t="s">
+      <c r="C277" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D277" s="82" t="s">
+      <c r="D277" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E277" s="89">
+      <c r="E277" s="88">
         <v>7</v>
       </c>
-      <c r="F277" s="90" t="s">
+      <c r="F277" s="89" t="s">
         <v>353</v>
       </c>
-      <c r="G277" s="82" t="s">
+      <c r="G277" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H277" s="82" t="s">
+      <c r="H277" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="J277" s="69"/>
+      <c r="J277" s="68"/>
     </row>
     <row r="278" spans="1:10" ht="14.3" customHeight="1">
-      <c r="A278" s="82" t="s">
+      <c r="A278" s="81" t="s">
         <v>316</v>
       </c>
-      <c r="B278" s="82" t="s">
+      <c r="B278" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C278" s="82" t="s">
+      <c r="C278" s="81" t="s">
         <v>345</v>
       </c>
-      <c r="D278" s="82" t="s">
+      <c r="D278" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="E278" s="89">
+      <c r="E278" s="88">
         <v>8</v>
       </c>
-      <c r="F278" s="90" t="s">
+      <c r="F278" s="89" t="s">
         <v>354</v>
       </c>
-      <c r="G278" s="82" t="s">
+      <c r="G278" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H278" s="82" t="s">
+      <c r="H278" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="J278" s="69"/>
+      <c r="J278" s="68"/>
     </row>
     <row r="279" spans="1:10" ht="14.3" customHeight="1">
       <c r="A279" s="4" t="s">
@@ -12103,7 +12150,7 @@
       <c r="B307" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C307" s="107" t="s">
+      <c r="C307" s="106" t="s">
         <v>379</v>
       </c>
       <c r="D307" s="4" t="s">
@@ -13143,54 +13190,54 @@
       </c>
     </row>
     <row r="348" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A348" s="82" t="s">
+      <c r="A348" s="81" t="s">
         <v>387</v>
       </c>
-      <c r="B348" s="82" t="s">
+      <c r="B348" s="81" t="s">
         <v>388</v>
       </c>
-      <c r="C348" s="87" t="s">
+      <c r="C348" s="86" t="s">
         <v>416</v>
       </c>
-      <c r="D348" s="88" t="s">
+      <c r="D348" s="87" t="s">
         <v>417</v>
       </c>
-      <c r="E348" s="89">
+      <c r="E348" s="88">
         <v>1</v>
       </c>
-      <c r="F348" s="90" t="s">
+      <c r="F348" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="G348" s="82" t="s">
+      <c r="G348" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H348" s="82" t="s">
+      <c r="H348" s="81" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="349" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A349" s="82" t="s">
+      <c r="A349" s="81" t="s">
         <v>387</v>
       </c>
-      <c r="B349" s="82" t="s">
+      <c r="B349" s="81" t="s">
         <v>388</v>
       </c>
-      <c r="C349" s="88" t="s">
+      <c r="C349" s="87" t="s">
         <v>416</v>
       </c>
-      <c r="D349" s="88" t="s">
+      <c r="D349" s="87" t="s">
         <v>417</v>
       </c>
-      <c r="E349" s="89">
+      <c r="E349" s="88">
         <v>2</v>
       </c>
-      <c r="F349" s="90" t="s">
+      <c r="F349" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="G349" s="82" t="s">
+      <c r="G349" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H349" s="82" t="s">
+      <c r="H349" s="81" t="s">
         <v>945</v>
       </c>
     </row>
@@ -14366,55 +14413,55 @@
         <v>471</v>
       </c>
     </row>
-    <row r="396" spans="1:8" s="69" customFormat="1" ht="14.3" customHeight="1">
-      <c r="A396" s="82" t="s">
+    <row r="396" spans="1:8" s="68" customFormat="1" ht="14.3" customHeight="1">
+      <c r="A396" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="B396" s="82" t="s">
+      <c r="B396" s="81" t="s">
         <v>435</v>
       </c>
-      <c r="C396" s="82" t="s">
+      <c r="C396" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="D396" s="82" t="s">
+      <c r="D396" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="E396" s="82" t="s">
+      <c r="E396" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F396" s="82" t="s">
+      <c r="F396" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="G396" s="82" t="s">
+      <c r="G396" s="81" t="s">
         <v>943</v>
       </c>
-      <c r="H396" s="82" t="s">
+      <c r="H396" s="81" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="397" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A397" s="82" t="s">
+      <c r="A397" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="B397" s="82" t="s">
+      <c r="B397" s="81" t="s">
         <v>435</v>
       </c>
-      <c r="C397" s="82" t="s">
+      <c r="C397" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="D397" s="82" t="s">
+      <c r="D397" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="E397" s="82" t="s">
+      <c r="E397" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F397" s="82" t="s">
+      <c r="F397" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="G397" s="82" t="s">
+      <c r="G397" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="H397" s="82" t="s">
+      <c r="H397" s="81" t="s">
         <v>112</v>
       </c>
     </row>
@@ -16235,106 +16282,106 @@
       </c>
     </row>
     <row r="468" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A468" s="71" t="s">
+      <c r="A468" s="70" t="s">
         <v>495</v>
       </c>
-      <c r="B468" s="71" t="s">
+      <c r="B468" s="70" t="s">
         <v>496</v>
       </c>
-      <c r="C468" s="72" t="s">
+      <c r="C468" s="71" t="s">
         <v>554</v>
       </c>
-      <c r="D468" s="71" t="s">
+      <c r="D468" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="E468" s="72">
+      <c r="E468" s="71">
         <v>1</v>
       </c>
-      <c r="F468" s="73" t="s">
+      <c r="F468" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="G468" s="71" t="s">
+      <c r="G468" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H468" s="71" t="s">
+      <c r="H468" s="70" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="469" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A469" s="71" t="s">
+      <c r="A469" s="70" t="s">
         <v>495</v>
       </c>
-      <c r="B469" s="71" t="s">
+      <c r="B469" s="70" t="s">
         <v>496</v>
       </c>
-      <c r="C469" s="72" t="s">
+      <c r="C469" s="71" t="s">
         <v>554</v>
       </c>
-      <c r="D469" s="71" t="s">
+      <c r="D469" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="E469" s="72">
+      <c r="E469" s="71">
         <v>2</v>
       </c>
-      <c r="F469" s="73" t="s">
+      <c r="F469" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="G469" s="71" t="s">
+      <c r="G469" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H469" s="71" t="s">
+      <c r="H469" s="70" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="470" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A470" s="71" t="s">
+      <c r="A470" s="70" t="s">
         <v>495</v>
       </c>
-      <c r="B470" s="71" t="s">
+      <c r="B470" s="70" t="s">
         <v>496</v>
       </c>
-      <c r="C470" s="72" t="s">
+      <c r="C470" s="71" t="s">
         <v>554</v>
       </c>
-      <c r="D470" s="71" t="s">
+      <c r="D470" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="E470" s="72">
+      <c r="E470" s="71">
         <v>88</v>
       </c>
-      <c r="F470" s="73" t="s">
+      <c r="F470" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="G470" s="71" t="s">
+      <c r="G470" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H470" s="71" t="s">
+      <c r="H470" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="471" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A471" s="71" t="s">
+      <c r="A471" s="70" t="s">
         <v>495</v>
       </c>
-      <c r="B471" s="71" t="s">
+      <c r="B471" s="70" t="s">
         <v>496</v>
       </c>
-      <c r="C471" s="72" t="s">
+      <c r="C471" s="71" t="s">
         <v>554</v>
       </c>
-      <c r="D471" s="71" t="s">
+      <c r="D471" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="E471" s="72">
+      <c r="E471" s="71">
         <v>99</v>
       </c>
-      <c r="F471" s="73" t="s">
+      <c r="F471" s="72" t="s">
         <v>557</v>
       </c>
-      <c r="G471" s="71" t="s">
+      <c r="G471" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H471" s="71" t="s">
+      <c r="H471" s="70" t="s">
         <v>30</v>
       </c>
     </row>
@@ -17754,54 +17801,54 @@
       </c>
     </row>
     <row r="526" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A526" s="71" t="s">
+      <c r="A526" s="70" t="s">
         <v>583</v>
       </c>
-      <c r="B526" s="71" t="s">
+      <c r="B526" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="C526" s="72" t="s">
+      <c r="C526" s="71" t="s">
         <v>622</v>
       </c>
-      <c r="D526" s="79" t="s">
+      <c r="D526" s="78" t="s">
         <v>623</v>
       </c>
-      <c r="E526" s="72">
+      <c r="E526" s="71">
         <v>1</v>
       </c>
-      <c r="F526" s="71" t="s">
+      <c r="F526" s="70" t="s">
         <v>621</v>
       </c>
-      <c r="G526" s="71" t="s">
+      <c r="G526" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H526" s="71" t="s">
+      <c r="H526" s="70" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="527" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A527" s="71" t="s">
+      <c r="A527" s="70" t="s">
         <v>583</v>
       </c>
-      <c r="B527" s="71" t="s">
+      <c r="B527" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="C527" s="72" t="s">
+      <c r="C527" s="71" t="s">
         <v>622</v>
       </c>
-      <c r="D527" s="79" t="s">
+      <c r="D527" s="78" t="s">
         <v>623</v>
       </c>
-      <c r="E527" s="72">
+      <c r="E527" s="71">
         <v>2</v>
       </c>
-      <c r="F527" s="71" t="s">
+      <c r="F527" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="G527" s="71" t="s">
+      <c r="G527" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H527" s="71" t="s">
+      <c r="H527" s="70" t="s">
         <v>556</v>
       </c>
     </row>
@@ -18980,10 +19027,10 @@
       <c r="F573" s="41" t="s">
         <v>669</v>
       </c>
-      <c r="G573" s="122" t="s">
+      <c r="G573" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="H573" s="123"/>
+      <c r="H573" s="125"/>
     </row>
     <row r="574" spans="1:8" ht="14.3" customHeight="1">
       <c r="A574" s="4" t="s">
@@ -19004,10 +19051,10 @@
       <c r="F574" s="41" t="s">
         <v>671</v>
       </c>
-      <c r="G574" s="122" t="s">
+      <c r="G574" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="H574" s="123"/>
+      <c r="H574" s="125"/>
     </row>
     <row r="575" spans="1:8" ht="14.3" customHeight="1">
       <c r="A575" s="4" t="s">
@@ -19112,54 +19159,54 @@
       </c>
     </row>
     <row r="579" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A579" s="74" t="s">
+      <c r="A579" s="73" t="s">
         <v>651</v>
       </c>
-      <c r="B579" s="74" t="s">
+      <c r="B579" s="73" t="s">
         <v>652</v>
       </c>
-      <c r="C579" s="75" t="s">
+      <c r="C579" s="74" t="s">
         <v>653</v>
       </c>
-      <c r="D579" s="74" t="s">
+      <c r="D579" s="73" t="s">
         <v>654</v>
       </c>
-      <c r="E579" s="75">
+      <c r="E579" s="74">
         <v>1</v>
       </c>
-      <c r="F579" s="74" t="s">
+      <c r="F579" s="73" t="s">
         <v>655</v>
       </c>
-      <c r="G579" s="74" t="s">
+      <c r="G579" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H579" s="74" t="s">
+      <c r="H579" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="580" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A580" s="74" t="s">
+      <c r="A580" s="73" t="s">
         <v>651</v>
       </c>
-      <c r="B580" s="74" t="s">
+      <c r="B580" s="73" t="s">
         <v>652</v>
       </c>
-      <c r="C580" s="75" t="s">
+      <c r="C580" s="74" t="s">
         <v>653</v>
       </c>
-      <c r="D580" s="74" t="s">
+      <c r="D580" s="73" t="s">
         <v>654</v>
       </c>
-      <c r="E580" s="75">
+      <c r="E580" s="74">
         <v>2</v>
       </c>
-      <c r="F580" s="74" t="s">
+      <c r="F580" s="73" t="s">
         <v>656</v>
       </c>
-      <c r="G580" s="74" t="s">
+      <c r="G580" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H580" s="74" t="s">
+      <c r="H580" s="73" t="s">
         <v>556</v>
       </c>
     </row>
@@ -20660,106 +20707,106 @@
       </c>
     </row>
     <row r="639" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A639" s="71" t="s">
+      <c r="A639" s="70" t="s">
         <v>700</v>
       </c>
-      <c r="B639" s="71" t="s">
+      <c r="B639" s="70" t="s">
         <v>701</v>
       </c>
-      <c r="C639" s="72" t="s">
+      <c r="C639" s="71" t="s">
         <v>740</v>
       </c>
-      <c r="D639" s="76" t="s">
+      <c r="D639" s="75" t="s">
         <v>741</v>
       </c>
-      <c r="E639" s="77">
+      <c r="E639" s="76">
         <v>1</v>
       </c>
-      <c r="F639" s="78" t="s">
+      <c r="F639" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="G639" s="71" t="s">
+      <c r="G639" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H639" s="71" t="s">
+      <c r="H639" s="70" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="640" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A640" s="71" t="s">
+      <c r="A640" s="70" t="s">
         <v>700</v>
       </c>
-      <c r="B640" s="71" t="s">
+      <c r="B640" s="70" t="s">
         <v>701</v>
       </c>
-      <c r="C640" s="72" t="s">
+      <c r="C640" s="71" t="s">
         <v>740</v>
       </c>
-      <c r="D640" s="76" t="s">
+      <c r="D640" s="75" t="s">
         <v>741</v>
       </c>
-      <c r="E640" s="77">
+      <c r="E640" s="76">
         <v>6</v>
       </c>
-      <c r="F640" s="78" t="s">
+      <c r="F640" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="G640" s="71" t="s">
+      <c r="G640" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H640" s="71" t="s">
+      <c r="H640" s="70" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="641" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A641" s="71" t="s">
+      <c r="A641" s="70" t="s">
         <v>700</v>
       </c>
-      <c r="B641" s="71" t="s">
+      <c r="B641" s="70" t="s">
         <v>701</v>
       </c>
-      <c r="C641" s="72" t="s">
+      <c r="C641" s="71" t="s">
         <v>740</v>
       </c>
-      <c r="D641" s="76" t="s">
+      <c r="D641" s="75" t="s">
         <v>741</v>
       </c>
-      <c r="E641" s="77">
+      <c r="E641" s="76">
         <v>9</v>
       </c>
-      <c r="F641" s="78" t="s">
+      <c r="F641" s="77" t="s">
         <v>714</v>
       </c>
-      <c r="G641" s="71" t="s">
+      <c r="G641" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H641" s="71" t="s">
+      <c r="H641" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="642" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A642" s="71" t="s">
+      <c r="A642" s="70" t="s">
         <v>700</v>
       </c>
-      <c r="B642" s="71" t="s">
+      <c r="B642" s="70" t="s">
         <v>701</v>
       </c>
-      <c r="C642" s="72" t="s">
+      <c r="C642" s="71" t="s">
         <v>740</v>
       </c>
-      <c r="D642" s="76" t="s">
+      <c r="D642" s="75" t="s">
         <v>741</v>
       </c>
-      <c r="E642" s="77" t="s">
+      <c r="E642" s="76" t="s">
         <v>731</v>
       </c>
-      <c r="F642" s="78" t="s">
+      <c r="F642" s="77" t="s">
         <v>264</v>
       </c>
-      <c r="G642" s="71" t="s">
+      <c r="G642" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H642" s="71" t="s">
+      <c r="H642" s="70" t="s">
         <v>30</v>
       </c>
     </row>
@@ -22292,54 +22339,54 @@
       </c>
     </row>
     <row r="702" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A702" s="71" t="s">
+      <c r="A702" s="70" t="s">
         <v>766</v>
       </c>
-      <c r="B702" s="71" t="s">
+      <c r="B702" s="70" t="s">
         <v>767</v>
       </c>
-      <c r="C702" s="72" t="s">
+      <c r="C702" s="71" t="s">
         <v>801</v>
       </c>
-      <c r="D702" s="70" t="s">
+      <c r="D702" s="69" t="s">
         <v>802</v>
       </c>
-      <c r="E702" s="72">
+      <c r="E702" s="71">
         <v>1</v>
       </c>
-      <c r="F702" s="71" t="s">
+      <c r="F702" s="70" t="s">
         <v>621</v>
       </c>
-      <c r="G702" s="71" t="s">
+      <c r="G702" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H702" s="71" t="s">
+      <c r="H702" s="70" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="703" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A703" s="71" t="s">
+      <c r="A703" s="70" t="s">
         <v>766</v>
       </c>
-      <c r="B703" s="71" t="s">
+      <c r="B703" s="70" t="s">
         <v>767</v>
       </c>
-      <c r="C703" s="72" t="s">
+      <c r="C703" s="71" t="s">
         <v>801</v>
       </c>
-      <c r="D703" s="70" t="s">
+      <c r="D703" s="69" t="s">
         <v>802</v>
       </c>
-      <c r="E703" s="72">
+      <c r="E703" s="71">
         <v>2</v>
       </c>
-      <c r="F703" s="71" t="s">
+      <c r="F703" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="G703" s="71" t="s">
+      <c r="G703" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="H703" s="71" t="s">
+      <c r="H703" s="70" t="s">
         <v>556</v>
       </c>
     </row>
@@ -22425,10 +22472,10 @@
       <c r="A707" s="4" t="s">
         <v>766</v>
       </c>
-      <c r="B707" s="122" t="s">
+      <c r="B707" s="124" t="s">
         <v>767</v>
       </c>
-      <c r="C707" s="123"/>
+      <c r="C707" s="125"/>
       <c r="D707" s="50" t="s">
         <v>806</v>
       </c>
@@ -22449,10 +22496,10 @@
       <c r="A708" s="4" t="s">
         <v>766</v>
       </c>
-      <c r="B708" s="122" t="s">
+      <c r="B708" s="124" t="s">
         <v>767</v>
       </c>
-      <c r="C708" s="123"/>
+      <c r="C708" s="125"/>
       <c r="D708" s="50" t="s">
         <v>806</v>
       </c>
@@ -23916,210 +23963,210 @@
       </c>
     </row>
     <row r="765" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A765" s="74" t="s">
+      <c r="A765" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B765" s="74" t="s">
+      <c r="B765" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C765" s="75" t="s">
+      <c r="C765" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D765" s="74" t="s">
+      <c r="D765" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E765" s="75">
+      <c r="E765" s="74">
         <v>1</v>
       </c>
-      <c r="F765" s="74" t="s">
+      <c r="F765" s="73" t="s">
         <v>865</v>
       </c>
-      <c r="G765" s="74" t="s">
+      <c r="G765" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H765" s="74" t="s">
+      <c r="H765" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="766" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A766" s="74" t="s">
+      <c r="A766" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B766" s="74" t="s">
+      <c r="B766" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C766" s="75" t="s">
+      <c r="C766" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D766" s="74" t="s">
+      <c r="D766" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E766" s="75">
+      <c r="E766" s="74">
         <v>2</v>
       </c>
-      <c r="F766" s="74" t="s">
+      <c r="F766" s="73" t="s">
         <v>866</v>
       </c>
-      <c r="G766" s="74" t="s">
+      <c r="G766" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H766" s="74" t="s">
+      <c r="H766" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="767" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A767" s="74" t="s">
+      <c r="A767" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B767" s="74" t="s">
+      <c r="B767" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C767" s="75" t="s">
+      <c r="C767" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D767" s="74" t="s">
+      <c r="D767" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E767" s="75">
+      <c r="E767" s="74">
         <v>3</v>
       </c>
-      <c r="F767" s="74" t="s">
+      <c r="F767" s="73" t="s">
         <v>867</v>
       </c>
-      <c r="G767" s="74" t="s">
+      <c r="G767" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H767" s="74" t="s">
+      <c r="H767" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="768" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A768" s="74" t="s">
+      <c r="A768" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B768" s="74" t="s">
+      <c r="B768" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C768" s="75" t="s">
+      <c r="C768" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D768" s="74" t="s">
+      <c r="D768" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E768" s="75">
+      <c r="E768" s="74">
         <v>4</v>
       </c>
-      <c r="F768" s="74" t="s">
+      <c r="F768" s="73" t="s">
         <v>868</v>
       </c>
-      <c r="G768" s="74" t="s">
+      <c r="G768" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H768" s="74" t="s">
+      <c r="H768" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="769" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A769" s="74" t="s">
+      <c r="A769" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B769" s="74" t="s">
+      <c r="B769" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C769" s="75" t="s">
+      <c r="C769" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D769" s="74" t="s">
+      <c r="D769" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E769" s="75">
+      <c r="E769" s="74">
         <v>5</v>
       </c>
-      <c r="F769" s="74" t="s">
+      <c r="F769" s="73" t="s">
         <v>869</v>
       </c>
-      <c r="G769" s="74" t="s">
+      <c r="G769" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H769" s="74" t="s">
+      <c r="H769" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="770" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A770" s="74" t="s">
+      <c r="A770" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B770" s="74" t="s">
+      <c r="B770" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C770" s="75" t="s">
+      <c r="C770" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D770" s="74" t="s">
+      <c r="D770" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E770" s="75">
+      <c r="E770" s="74">
         <v>6</v>
       </c>
-      <c r="F770" s="74" t="s">
+      <c r="F770" s="73" t="s">
         <v>870</v>
       </c>
-      <c r="G770" s="74" t="s">
+      <c r="G770" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H770" s="74" t="s">
+      <c r="H770" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="771" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A771" s="74" t="s">
+      <c r="A771" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B771" s="74" t="s">
+      <c r="B771" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C771" s="75" t="s">
+      <c r="C771" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D771" s="74" t="s">
+      <c r="D771" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E771" s="75">
+      <c r="E771" s="74">
         <v>7</v>
       </c>
-      <c r="F771" s="74" t="s">
+      <c r="F771" s="73" t="s">
         <v>871</v>
       </c>
-      <c r="G771" s="74" t="s">
+      <c r="G771" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H771" s="74" t="s">
+      <c r="H771" s="73" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="772" spans="1:8" ht="14.3" customHeight="1">
-      <c r="A772" s="74" t="s">
+      <c r="A772" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="B772" s="74" t="s">
+      <c r="B772" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C772" s="75" t="s">
+      <c r="C772" s="74" t="s">
         <v>863</v>
       </c>
-      <c r="D772" s="74" t="s">
+      <c r="D772" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="E772" s="75">
+      <c r="E772" s="74">
         <v>8</v>
       </c>
-      <c r="F772" s="74" t="s">
+      <c r="F772" s="73" t="s">
         <v>842</v>
       </c>
-      <c r="G772" s="74" t="s">
+      <c r="G772" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="H772" s="74" t="s">
+      <c r="H772" s="73" t="s">
         <v>738</v>
       </c>
     </row>
@@ -24315,10 +24362,10 @@
       <c r="C780" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="D780" s="122" t="s">
+      <c r="D780" s="124" t="s">
         <v>882</v>
       </c>
-      <c r="E780" s="123"/>
+      <c r="E780" s="125"/>
       <c r="F780" s="52">
         <v>0.47222222222222221</v>
       </c>
@@ -24365,10 +24412,10 @@
       <c r="C782" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="D782" s="122" t="s">
+      <c r="D782" s="124" t="s">
         <v>884</v>
       </c>
-      <c r="E782" s="123"/>
+      <c r="E782" s="125"/>
       <c r="F782" s="53">
         <v>17.290972222222223</v>
       </c>
@@ -24389,10 +24436,10 @@
       <c r="C783" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="D783" s="122" t="s">
+      <c r="D783" s="124" t="s">
         <v>884</v>
       </c>
-      <c r="E783" s="123"/>
+      <c r="E783" s="125"/>
       <c r="F783" s="53">
         <v>4.4437499999999996</v>
       </c>
@@ -25432,17 +25479,17 @@
   </sheetData>
   <autoFilter ref="A1:H788" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="11">
-    <mergeCell ref="G573:H573"/>
-    <mergeCell ref="G574:H574"/>
-    <mergeCell ref="B707:C707"/>
-    <mergeCell ref="B708:C708"/>
-    <mergeCell ref="D780:E780"/>
     <mergeCell ref="D782:E782"/>
     <mergeCell ref="D783:E783"/>
     <mergeCell ref="D56:F56"/>
     <mergeCell ref="D57:F57"/>
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="D59:F59"/>
+    <mergeCell ref="G573:H573"/>
+    <mergeCell ref="G574:H574"/>
+    <mergeCell ref="B707:C707"/>
+    <mergeCell ref="B708:C708"/>
+    <mergeCell ref="D780:E780"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -25451,10 +25498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:D39"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.95" customHeight="1"/>
@@ -25657,7 +25704,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.3" customHeight="1">
+    <row r="17" spans="1:5" ht="14.3" customHeight="1">
       <c r="A17" s="54">
         <v>16</v>
       </c>
@@ -25668,7 +25715,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.3" customHeight="1">
+    <row r="18" spans="1:5" ht="14.3" customHeight="1">
       <c r="A18" s="54">
         <v>17</v>
       </c>
@@ -25679,7 +25726,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.3" customHeight="1">
+    <row r="19" spans="1:5" ht="14.3" customHeight="1">
       <c r="A19" s="54">
         <v>18</v>
       </c>
@@ -25690,7 +25737,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.3" customHeight="1">
+    <row r="20" spans="1:5" ht="14.3" customHeight="1">
       <c r="A20" s="54">
         <v>19</v>
       </c>
@@ -25704,19 +25751,19 @@
         <v>921</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.3" customHeight="1">
+    <row r="21" spans="1:5" ht="14.3" customHeight="1">
       <c r="A21" s="54"/>
       <c r="B21" s="54"/>
     </row>
-    <row r="22" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="23" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="24" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="25" spans="1:4" ht="14.3" customHeight="1">
+    <row r="22" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="23" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="24" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="25" spans="1:5" ht="14.3" customHeight="1">
       <c r="A25" s="60" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.3" customHeight="1">
+    <row r="26" spans="1:5" ht="14.3" customHeight="1">
       <c r="A26" s="61" t="s">
         <v>923</v>
       </c>
@@ -25729,8 +25776,11 @@
       <c r="D26" s="65" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E26" s="130" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.3" customHeight="1">
       <c r="A27" s="60" t="s">
         <v>925</v>
       </c>
@@ -25741,7 +25791,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.3" customHeight="1">
+    <row r="28" spans="1:5" ht="14.3" customHeight="1">
       <c r="A28" s="60" t="s">
         <v>583</v>
       </c>
@@ -25752,7 +25802,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.3" customHeight="1">
+    <row r="29" spans="1:5" ht="14.3" customHeight="1">
       <c r="A29" s="60" t="s">
         <v>651</v>
       </c>
@@ -25763,7 +25813,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.3" customHeight="1">
+    <row r="30" spans="1:5" ht="14.3" customHeight="1">
       <c r="A30" s="60" t="s">
         <v>700</v>
       </c>
@@ -25774,7 +25824,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.3" customHeight="1">
+    <row r="31" spans="1:5" ht="14.3" customHeight="1">
       <c r="A31" s="60" t="s">
         <v>766</v>
       </c>
@@ -25785,7 +25835,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.3" customHeight="1">
+    <row r="32" spans="1:5" ht="14.3" customHeight="1">
       <c r="A32" s="60" t="s">
         <v>931</v>
       </c>
@@ -25796,7 +25846,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.3" customHeight="1">
+    <row r="33" spans="1:5" ht="14.3" customHeight="1">
       <c r="A33" s="16" t="s">
         <v>8</v>
       </c>
@@ -25809,8 +25859,11 @@
       <c r="D33" s="64" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E33" s="123" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.3" customHeight="1">
       <c r="A34" s="16" t="s">
         <v>108</v>
       </c>
@@ -25823,8 +25876,11 @@
       <c r="D34" s="64" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E34" s="64" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.3" customHeight="1">
       <c r="A35" s="16" t="s">
         <v>188</v>
       </c>
@@ -25834,19 +25890,25 @@
       <c r="C35" s="66" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E35" s="64" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.3" customHeight="1">
       <c r="A36" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="B36" s="67" t="s">
+      <c r="B36" s="54" t="s">
         <v>282</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E36" s="64" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.3" customHeight="1">
       <c r="A37" s="16" t="s">
         <v>316</v>
       </c>
@@ -25856,8 +25918,11 @@
       <c r="C37" s="16" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E37" s="64" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.3" customHeight="1">
       <c r="A38" s="16" t="s">
         <v>387</v>
       </c>
@@ -25867,8 +25932,11 @@
       <c r="C38" s="16" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="14.3" customHeight="1">
+      <c r="E38" s="64" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.3" customHeight="1">
       <c r="A39" s="16" t="s">
         <v>434</v>
       </c>
@@ -25881,16 +25949,35 @@
       <c r="D39" s="64" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="41" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="42" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="43" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="44" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="45" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="46" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="47" spans="1:4" ht="14.3" customHeight="1"/>
-    <row r="48" spans="1:4" ht="14.3" customHeight="1"/>
+      <c r="E39" s="64" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.3" customHeight="1">
+      <c r="A40" s="123" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C40" s="123" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E40" s="123" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="42" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="43" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="44" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="45" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="46" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="47" spans="1:5" ht="14.3" customHeight="1"/>
+    <row r="48" spans="1:5" ht="14.3" customHeight="1"/>
     <row r="49" ht="14.3" customHeight="1"/>
     <row r="50" ht="14.3" customHeight="1"/>
     <row r="51" ht="14.3" customHeight="1"/>
@@ -26853,569 +26940,571 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E39F68A-D908-4889-A868-9822F377BC18}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="93"/>
-    <col min="3" max="3" width="14.109375" style="93" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" style="93" customWidth="1"/>
-    <col min="5" max="5" width="70.33203125" style="93" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="93" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="93" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="93"/>
+    <col min="1" max="2" width="11.5546875" style="92"/>
+    <col min="3" max="3" width="14.109375" style="92" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="92" customWidth="1"/>
+    <col min="5" max="5" width="70.33203125" style="92" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="92" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="92" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="92"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="91" t="s">
         <v>923</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="91" t="s">
         <v>957</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="91" t="s">
         <v>958</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="91" t="s">
         <v>959</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="91" t="s">
         <v>960</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="91" t="s">
         <v>961</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="91" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>931</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="92" t="s">
         <v>963</v>
       </c>
-      <c r="C2" s="93">
+      <c r="C2" s="92">
         <v>164</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="92" t="s">
         <v>964</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="92" t="s">
         <v>965</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="92" t="s">
         <v>931</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="92" t="s">
         <v>966</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="92">
         <v>230</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="92" t="s">
         <v>967</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="92" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>495</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="92" t="s">
         <v>968</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="92">
         <v>17</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="92" t="s">
         <v>969</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>970</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="92" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="92" t="s">
         <v>495</v>
       </c>
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="92" t="s">
         <v>971</v>
       </c>
-      <c r="C5" s="93">
+      <c r="C5" s="92">
         <v>21</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="92" t="s">
         <v>972</v>
       </c>
-      <c r="E5" s="93" t="s">
+      <c r="E5" s="92" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="92" t="s">
         <v>583</v>
       </c>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="92" t="s">
         <v>974</v>
       </c>
-      <c r="C6" s="93">
+      <c r="C6" s="92">
         <v>609</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="92" t="s">
         <v>975</v>
       </c>
-      <c r="E6" s="93" t="s">
+      <c r="E6" s="92" t="s">
         <v>976</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="92" t="s">
         <v>700</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="92" t="s">
         <v>764</v>
       </c>
-      <c r="C7" s="93">
+      <c r="C7" s="92">
         <v>594</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="92" t="s">
         <v>977</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="92" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="92" t="s">
         <v>700</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="92" t="s">
         <v>978</v>
       </c>
-      <c r="C8" s="93">
+      <c r="C8" s="92">
         <v>292</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="D8" s="92" t="s">
         <v>979</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="92" t="s">
         <v>980</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="G8" s="92" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="92" t="s">
         <v>651</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="92" t="s">
         <v>981</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="92">
         <v>423</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="92" t="s">
         <v>982</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="92" t="s">
         <v>983</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="92" t="s">
         <v>890</v>
       </c>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="92" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="92" t="s">
         <v>651</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="92" t="s">
         <v>984</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="92">
         <v>436</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="92" t="s">
         <v>985</v>
       </c>
-      <c r="E10" s="93" t="s">
+      <c r="E10" s="92" t="s">
         <v>986</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="92" t="s">
         <v>890</v>
       </c>
-      <c r="G10" s="93" t="s">
+      <c r="G10" s="92" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="92" t="s">
         <v>766</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="93" t="s">
         <v>987</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="92" t="s">
         <v>988</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="D11" s="92" t="s">
         <v>989</v>
       </c>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="94" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="92" t="s">
         <v>766</v>
       </c>
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="95" t="s">
         <v>991</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="92" t="s">
         <v>992</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="92" t="s">
         <v>434</v>
       </c>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="92" t="s">
         <v>493</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="122" t="s">
         <v>494</v>
       </c>
-      <c r="E13" s="93" t="s">
+      <c r="E13" s="92" t="s">
         <v>993</v>
       </c>
-      <c r="F13" s="93" t="s">
+      <c r="F13" s="92" t="s">
         <v>994</v>
       </c>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="92" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="40.75" customHeight="1">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="96" t="s">
         <v>996</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="96" t="s">
         <v>997</v>
       </c>
-      <c r="F14" s="98" t="s">
+      <c r="F14" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G14" s="93" t="s">
+      <c r="G14" s="92" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="92" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="93">
+      <c r="C15" s="92">
         <v>45</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="92" t="s">
         <v>998</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="G15" s="92" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="92" t="s">
         <v>250</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="98" t="s">
         <v>999</v>
       </c>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="92" t="s">
         <v>1000</v>
       </c>
-      <c r="E16" s="93" t="s">
+      <c r="E16" s="92" t="s">
         <v>1001</v>
       </c>
-      <c r="F16" s="98" t="s">
+      <c r="F16" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G16" s="99" t="s">
+      <c r="G16" s="98" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.55">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="92" t="s">
         <v>252</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="99" t="s">
         <v>1002</v>
       </c>
-      <c r="E17" s="100" t="s">
+      <c r="E17" s="99" t="s">
         <v>1003</v>
       </c>
-      <c r="F17" s="98" t="s">
+      <c r="F17" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G17" s="93" t="s">
+      <c r="G17" s="92" t="s">
         <v>1004</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="95" t="s">
         <v>426</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="92" t="s">
         <v>427</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="92" t="s">
         <v>1005</v>
       </c>
-      <c r="F18" s="98" t="s">
+      <c r="F18" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="97" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="95" t="s">
         <v>428</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="92" t="s">
         <v>429</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="92" t="s">
         <v>1006</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="100" t="s">
         <v>1007</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="95" t="s">
         <v>430</v>
       </c>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="92" t="s">
         <v>431</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="92" t="s">
         <v>1008</v>
       </c>
-      <c r="F20" s="98" t="s">
+      <c r="F20" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G20" s="101" t="s">
+      <c r="G20" s="100" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="95" t="s">
         <v>432</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="92" t="s">
         <v>433</v>
       </c>
-      <c r="E21" s="93" t="s">
+      <c r="E21" s="92" t="s">
         <v>1010</v>
       </c>
-      <c r="F21" s="98" t="s">
+      <c r="F21" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G21" s="101" t="s">
+      <c r="G21" s="100" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="100" t="s">
         <v>1012</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="95" t="s">
         <v>1013</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="92" t="s">
         <v>1014</v>
       </c>
-      <c r="F22" s="98" t="s">
+      <c r="F22" s="97" t="s">
         <v>890</v>
       </c>
-      <c r="G22" s="101" t="s">
+      <c r="G22" s="100" t="s">
         <v>1007</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="93" t="s">
+      <c r="A23" s="92" t="s">
         <v>1015</v>
       </c>
-      <c r="B23" s="102" t="s">
+      <c r="B23" s="101" t="s">
         <v>1016</v>
       </c>
-      <c r="D23" s="103" t="s">
+      <c r="D23" s="102" t="s">
         <v>1017</v>
       </c>
-      <c r="E23" s="93" t="s">
+      <c r="E23" s="92" t="s">
         <v>1018</v>
       </c>
-      <c r="F23" s="98" t="s">
+      <c r="F23" s="97" t="s">
         <v>1019</v>
       </c>
-      <c r="G23" s="101" t="s">
+      <c r="G23" s="100" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="92" t="s">
         <v>1015</v>
       </c>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="102" t="s">
         <v>1021</v>
       </c>
-      <c r="D24" s="103" t="s">
+      <c r="D24" s="102" t="s">
         <v>1022</v>
       </c>
-      <c r="E24" s="93" t="s">
+      <c r="E24" s="92" t="s">
         <v>1023</v>
       </c>
-      <c r="F24" s="98" t="s">
+      <c r="F24" s="97" t="s">
         <v>1019</v>
       </c>
-      <c r="G24" s="101" t="s">
+      <c r="G24" s="100" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.3" customHeight="1">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="92" t="s">
         <v>1024</v>
       </c>
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="102" t="s">
         <v>1025</v>
       </c>
-      <c r="C25" s="93">
+      <c r="C25" s="92">
         <v>19</v>
       </c>
-      <c r="D25" s="103" t="s">
+      <c r="D25" s="102" t="s">
         <v>1026</v>
       </c>
-      <c r="E25" s="97" t="s">
+      <c r="E25" s="96" t="s">
         <v>1027</v>
       </c>
-      <c r="F25" s="104" t="s">
+      <c r="F25" s="103" t="s">
         <v>890</v>
       </c>
-      <c r="G25" s="105" t="s">
+      <c r="G25" s="104" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="92" t="s">
         <v>316</v>
       </c>
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="92" t="s">
         <v>375</v>
       </c>
-      <c r="D26" s="93" t="s">
+      <c r="D26" s="92" t="s">
         <v>376</v>
       </c>
-      <c r="F26" s="104" t="s">
+      <c r="F26" s="103" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="92" t="s">
         <v>316</v>
       </c>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="92" t="s">
         <v>1028</v>
       </c>
-      <c r="D27" s="93" t="s">
+      <c r="D27" s="92" t="s">
         <v>1029</v>
       </c>
-      <c r="E27" s="93" t="s">
+      <c r="E27" s="92" t="s">
         <v>1030</v>
       </c>
-      <c r="F27" s="104" t="s">
+      <c r="F27" s="103" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="93" t="s">
+      <c r="A28" s="92" t="s">
         <v>316</v>
       </c>
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="92" t="s">
         <v>385</v>
       </c>
-      <c r="D28" s="93" t="s">
+      <c r="D28" s="92" t="s">
         <v>1031</v>
       </c>
-      <c r="E28" s="93" t="s">
+      <c r="E28" s="92" t="s">
         <v>1032</v>
       </c>
-      <c r="G28" s="105" t="s">
+      <c r="G28" s="104" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="92" t="s">
         <v>257</v>
       </c>
-      <c r="B29" s="93" t="s">
+      <c r="B29" s="92" t="s">
         <v>313</v>
       </c>
-      <c r="D29" s="93" t="s">
+      <c r="D29" s="92" t="s">
         <v>1033</v>
       </c>
-      <c r="E29" s="93" t="s">
+      <c r="E29" s="92" t="s">
         <v>1034</v>
       </c>
-      <c r="F29" s="104" t="s">
+      <c r="F29" s="103" t="s">
         <v>890</v>
       </c>
-      <c r="G29" s="105" t="s">
+      <c r="G29" s="104" t="s">
         <v>254</v>
       </c>
     </row>
@@ -27432,19 +27521,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805967D9-A16C-4BAC-B7E7-6A55F3D3D74A}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.6"/>
   <cols>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="121" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.95" thickBot="1">
+    <row r="1" spans="1:5" ht="14.95" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>923</v>
       </c>
@@ -27452,171 +27542,201 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.6" customHeight="1" thickTop="1">
+      <c r="A2" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>1035</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.6" customHeight="1" thickTop="1">
-      <c r="A2" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A3" s="80" t="s">
+      <c r="D2" s="121" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A3" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>109</v>
       </c>
       <c r="C3" s="64" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="D3" s="105" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A4" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>189</v>
       </c>
       <c r="C4" s="64" t="s">
         <v>1019</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A5" s="80" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A5" s="79" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="105" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E5" t="s">
         <v>1065</v>
       </c>
-      <c r="D5" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A6" s="80" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A6" s="79" t="s">
         <v>316</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>189</v>
       </c>
       <c r="C6" s="64" t="s">
         <v>1019</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A7" s="80" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A7" s="79" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="90" t="s">
         <v>388</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A8" s="80" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A8" s="79" t="s">
         <v>434</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="90" t="s">
         <v>435</v>
       </c>
       <c r="C8" s="64" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A9" s="80" t="s">
+      <c r="D8" s="64" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A9" s="79" t="s">
         <v>495</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="90" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A10" s="80" t="s">
+    <row r="10" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A10" s="79" t="s">
         <v>583</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A11" s="80" t="s">
+    <row r="11" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A11" s="79" t="s">
         <v>651</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="90" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A12" s="80" t="s">
+    <row r="12" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A12" s="79" t="s">
         <v>700</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="90" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A13" s="93" t="s">
+    <row r="13" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A13" s="92" t="s">
         <v>931</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="90" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A14" s="81" t="s">
+    <row r="14" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A14" s="80" t="s">
         <v>1012</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="90" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A15" s="79" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B15" s="90" t="s">
         <v>1037</v>
-      </c>
-      <c r="C14" s="81" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A15" s="80" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B15" s="91" t="s">
-        <v>1038</v>
       </c>
       <c r="C15" s="64" t="s">
         <v>890</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="13.6" customHeight="1">
-      <c r="A16" s="80" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="13.6" customHeight="1">
+      <c r="A16" s="79" t="s">
         <v>766</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="90" t="s">
         <v>767</v>
       </c>
     </row>
@@ -27631,143 +27751,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F73259B-4B92-4779-941C-4A0C4539E183}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="109" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" style="109" customWidth="1"/>
-    <col min="3" max="5" width="52.5546875" style="109" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="108"/>
+    <col min="1" max="1" width="32.6640625" style="108" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" style="108" customWidth="1"/>
+    <col min="3" max="5" width="52.5546875" style="108" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="107"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.55" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="126" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D1" s="126" t="s">
         <v>1043</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="E1" s="126" t="s">
         <v>1044</v>
       </c>
-      <c r="E1" s="124" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="20.55" customHeight="1">
+      <c r="A2" s="127"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+    </row>
+    <row r="3" spans="1:5" ht="30.1" customHeight="1" thickBot="1">
+      <c r="A3" s="109" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="111" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20.55" customHeight="1">
-      <c r="A2" s="125"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-    </row>
-    <row r="3" spans="1:5" ht="30.1" customHeight="1" thickBot="1">
-      <c r="A3" s="110" t="s">
-        <v>188</v>
-      </c>
-      <c r="B3" s="111" t="s">
+      <c r="D3" s="112" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="54.2" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D4" s="115" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E4" s="116" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30.1" customHeight="1" thickTop="1">
+      <c r="A5" s="117" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B5" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="117" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D5" s="117" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E5" s="117" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30.1" customHeight="1" thickBot="1">
+      <c r="A6" s="109" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="110" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="112" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D3" s="113" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E3" s="112" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="54.2" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="115" t="s">
-        <v>257</v>
-      </c>
-      <c r="B4" s="115" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="114" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D4" s="116" t="s">
-        <v>1050</v>
-      </c>
-      <c r="E4" s="117" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30.1" customHeight="1" thickTop="1">
-      <c r="A5" s="118" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B5" s="118" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="118" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D5" s="118" t="s">
-        <v>1053</v>
-      </c>
-      <c r="E5" s="118" t="s">
+      <c r="C6" s="111" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.1" customHeight="1" thickBot="1">
-      <c r="A6" s="110" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6" s="111" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="112" t="s">
+      <c r="D6" s="112" t="s">
         <v>1055</v>
       </c>
-      <c r="D6" s="113" t="s">
+      <c r="E6" s="111" t="s">
         <v>1056</v>
       </c>
-      <c r="E6" s="112" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="30.1" customHeight="1" thickTop="1">
+      <c r="A7" s="117" t="s">
         <v>1057</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30.1" customHeight="1" thickTop="1">
-      <c r="A7" s="118" t="s">
+      <c r="B7" s="117" t="s">
         <v>1058</v>
       </c>
-      <c r="B7" s="118" t="s">
+      <c r="C7" s="117" t="s">
         <v>1059</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="D7" s="117" t="s">
         <v>1060</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="E7" s="117" t="s">
         <v>1061</v>
       </c>
-      <c r="E7" s="118" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="56.4" customHeight="1">
+      <c r="A8" s="109" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8" s="118" t="s">
+        <v>435</v>
+      </c>
+      <c r="C8" s="119"/>
+      <c r="D8" s="120" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="56.4" customHeight="1">
-      <c r="A8" s="110" t="s">
-        <v>434</v>
-      </c>
-      <c r="B8" s="119" t="s">
-        <v>435</v>
-      </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="121" t="s">
+      <c r="E8" s="118" t="s">
         <v>1063</v>
-      </c>
-      <c r="E8" s="119" t="s">
-        <v>1064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primera ronda bases completas GW
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Guido\Trabajo\Economia\Tematicas de Investigacion\Precariedad Mundial\precariedad.mundial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB66B56E-7D59-4934-BD76-1DCFA296BF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6AA255-4813-47C2-9912-9DB527E4D8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -5106,8 +5106,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA1065"/>
   <sheetViews>
-    <sheetView topLeftCell="A864" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H871" sqref="H871"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B297" sqref="B193:B297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8731,7 +8731,7 @@
       </c>
       <c r="I132" s="4"/>
     </row>
-    <row r="133" spans="1:9" ht="14.25" hidden="1" customHeight="1" thickTop="1">
+    <row r="133" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A133" s="4" t="s">
         <v>186</v>
       </c>
@@ -10479,11 +10479,13 @@
         <v>258</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="13.5" hidden="1" customHeight="1">
+    <row r="193" spans="1:9" ht="13.5" customHeight="1" thickTop="1">
       <c r="A193" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B193" s="4"/>
+      <c r="B193" s="4">
+        <v>2019</v>
+      </c>
       <c r="C193" s="4" t="s">
         <v>260</v>
       </c>
@@ -10506,11 +10508,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="194" spans="1:9" ht="14.25" customHeight="1">
       <c r="A194" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B194" s="4"/>
+      <c r="B194" s="4">
+        <v>2019</v>
+      </c>
       <c r="C194" s="4" t="s">
         <v>260</v>
       </c>
@@ -10533,11 +10537,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="195" spans="1:9" ht="14.25" customHeight="1">
       <c r="A195" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B195" s="4"/>
+      <c r="B195" s="4">
+        <v>2019</v>
+      </c>
       <c r="C195" s="4" t="s">
         <v>260</v>
       </c>
@@ -10560,11 +10566,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="196" spans="1:9" ht="14.25" customHeight="1">
       <c r="A196" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B196" s="4"/>
+      <c r="B196" s="4">
+        <v>2019</v>
+      </c>
       <c r="C196" s="4" t="s">
         <v>260</v>
       </c>
@@ -10587,11 +10595,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="197" spans="1:9" ht="14.25" customHeight="1">
       <c r="A197" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B197" s="4"/>
+      <c r="B197" s="4">
+        <v>2019</v>
+      </c>
       <c r="C197" s="4" t="s">
         <v>260</v>
       </c>
@@ -10614,11 +10624,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="198" spans="1:9" ht="14.25" customHeight="1">
       <c r="A198" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B198" s="4"/>
+      <c r="B198" s="4">
+        <v>2019</v>
+      </c>
       <c r="C198" s="4" t="s">
         <v>260</v>
       </c>
@@ -10641,11 +10653,13 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="199" spans="1:9" ht="14.25" customHeight="1">
       <c r="A199" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B199" s="4"/>
+      <c r="B199" s="4">
+        <v>2019</v>
+      </c>
       <c r="C199" s="4" t="s">
         <v>260</v>
       </c>
@@ -10668,11 +10682,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="200" spans="1:9" ht="14.25" customHeight="1">
       <c r="A200" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B200" s="4"/>
+      <c r="B200" s="4">
+        <v>2019</v>
+      </c>
       <c r="C200" s="4" t="s">
         <v>260</v>
       </c>
@@ -10695,11 +10711,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="201" spans="1:9" ht="14.25" customHeight="1">
       <c r="A201" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B201" s="4"/>
+      <c r="B201" s="4">
+        <v>2019</v>
+      </c>
       <c r="C201" s="4" t="s">
         <v>260</v>
       </c>
@@ -10722,11 +10740,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="202" spans="1:9" ht="14.25" customHeight="1">
       <c r="A202" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B202" s="4"/>
+      <c r="B202" s="4">
+        <v>2019</v>
+      </c>
       <c r="C202" s="4" t="s">
         <v>260</v>
       </c>
@@ -10749,11 +10769,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="203" spans="1:9" ht="14.25" customHeight="1">
       <c r="A203" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B203" s="4"/>
+      <c r="B203" s="4">
+        <v>2019</v>
+      </c>
       <c r="C203" s="4" t="s">
         <v>260</v>
       </c>
@@ -10776,11 +10798,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="204" spans="1:9" ht="14.25" customHeight="1">
       <c r="A204" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B204" s="4"/>
+      <c r="B204" s="4">
+        <v>2019</v>
+      </c>
       <c r="C204" s="4" t="s">
         <v>260</v>
       </c>
@@ -10803,11 +10827,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="205" spans="1:9" ht="14.25" customHeight="1">
       <c r="A205" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B205" s="4"/>
+      <c r="B205" s="4">
+        <v>2019</v>
+      </c>
       <c r="C205" s="4" t="s">
         <v>260</v>
       </c>
@@ -10830,11 +10856,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="206" spans="1:9" ht="14.25" customHeight="1">
       <c r="A206" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B206" s="4"/>
+      <c r="B206" s="4">
+        <v>2019</v>
+      </c>
       <c r="C206" s="4" t="s">
         <v>260</v>
       </c>
@@ -10857,11 +10885,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="207" spans="1:9" ht="14.25" customHeight="1">
       <c r="A207" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B207" s="4"/>
+      <c r="B207" s="4">
+        <v>2019</v>
+      </c>
       <c r="C207" s="4" t="s">
         <v>260</v>
       </c>
@@ -10881,14 +10911,16 @@
         <v>1280</v>
       </c>
       <c r="I207" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="14.25" customHeight="1">
       <c r="A208" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B208" s="4"/>
+      <c r="B208" s="4">
+        <v>2019</v>
+      </c>
       <c r="C208" s="4" t="s">
         <v>260</v>
       </c>
@@ -10911,11 +10943,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="209" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="209" spans="1:27" ht="14.25" customHeight="1">
       <c r="A209" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B209" s="4"/>
+      <c r="B209" s="4">
+        <v>2019</v>
+      </c>
       <c r="C209" s="4" t="s">
         <v>260</v>
       </c>
@@ -10935,14 +10969,16 @@
         <v>1280</v>
       </c>
       <c r="I209" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="210" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="210" spans="1:27" ht="14.25" customHeight="1">
       <c r="A210" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B210" s="4"/>
+      <c r="B210" s="4">
+        <v>2019</v>
+      </c>
       <c r="C210" s="4" t="s">
         <v>260</v>
       </c>
@@ -10962,14 +10998,16 @@
         <v>1280</v>
       </c>
       <c r="I210" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="211" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="211" spans="1:27" ht="14.25" customHeight="1">
       <c r="A211" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B211" s="4"/>
+      <c r="B211" s="4">
+        <v>2019</v>
+      </c>
       <c r="C211" s="4" t="s">
         <v>260</v>
       </c>
@@ -10989,14 +11027,16 @@
         <v>1280</v>
       </c>
       <c r="I211" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="212" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="212" spans="1:27" ht="14.25" customHeight="1">
       <c r="A212" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B212" s="4"/>
+      <c r="B212" s="4">
+        <v>2019</v>
+      </c>
       <c r="C212" s="4" t="s">
         <v>260</v>
       </c>
@@ -11019,11 +11059,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="213" spans="1:27" ht="14.25" customHeight="1">
       <c r="A213" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B213" s="4"/>
+      <c r="B213" s="4">
+        <v>2019</v>
+      </c>
       <c r="C213" s="4" t="s">
         <v>260</v>
       </c>
@@ -11043,14 +11085,16 @@
         <v>1280</v>
       </c>
       <c r="I213" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="214" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="214" spans="1:27" ht="14.25" customHeight="1">
       <c r="A214" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B214" s="4"/>
+      <c r="B214" s="4">
+        <v>2019</v>
+      </c>
       <c r="C214" s="4" t="s">
         <v>260</v>
       </c>
@@ -11073,11 +11117,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="215" spans="1:27" ht="14.25" customHeight="1">
       <c r="A215" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B215" s="4"/>
+      <c r="B215" s="4">
+        <v>2019</v>
+      </c>
       <c r="C215" s="4" t="s">
         <v>260</v>
       </c>
@@ -11100,11 +11146,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="216" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="216" spans="1:27" ht="14.25" customHeight="1">
       <c r="A216" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B216" s="4"/>
+      <c r="B216" s="4">
+        <v>2019</v>
+      </c>
       <c r="C216" s="4" t="s">
         <v>260</v>
       </c>
@@ -11127,11 +11175,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="217" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="217" spans="1:27" ht="14.25" customHeight="1">
       <c r="A217" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B217" s="4"/>
+      <c r="B217" s="4">
+        <v>2019</v>
+      </c>
       <c r="C217" s="4" t="s">
         <v>260</v>
       </c>
@@ -11154,11 +11204,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="218" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="218" spans="1:27" ht="14.25" customHeight="1">
       <c r="A218" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B218" s="4"/>
+      <c r="B218" s="4">
+        <v>2019</v>
+      </c>
       <c r="C218" s="4" t="s">
         <v>260</v>
       </c>
@@ -11181,11 +11233,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="219" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="219" spans="1:27" ht="14.25" customHeight="1">
       <c r="A219" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B219" s="4"/>
+      <c r="B219" s="4">
+        <v>2019</v>
+      </c>
       <c r="C219" s="4" t="s">
         <v>260</v>
       </c>
@@ -11206,11 +11260,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="220" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="220" spans="1:27" ht="14.25" customHeight="1">
       <c r="A220" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B220" s="4"/>
+      <c r="B220" s="4">
+        <v>2019</v>
+      </c>
       <c r="C220" s="4" t="s">
         <v>260</v>
       </c>
@@ -11251,11 +11307,13 @@
       <c r="Z220" s="7"/>
       <c r="AA220" s="7"/>
     </row>
-    <row r="221" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="221" spans="1:27" ht="14.25" customHeight="1">
       <c r="A221" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B221" s="4"/>
+      <c r="B221" s="4">
+        <v>2019</v>
+      </c>
       <c r="C221" s="4" t="s">
         <v>260</v>
       </c>
@@ -11296,11 +11354,13 @@
       <c r="Z221" s="7"/>
       <c r="AA221" s="7"/>
     </row>
-    <row r="222" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="222" spans="1:27" ht="14.25" customHeight="1">
       <c r="A222" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B222" s="4"/>
+      <c r="B222" s="4">
+        <v>2019</v>
+      </c>
       <c r="C222" s="4" t="s">
         <v>260</v>
       </c>
@@ -11341,11 +11401,13 @@
       <c r="Z222" s="7"/>
       <c r="AA222" s="7"/>
     </row>
-    <row r="223" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="223" spans="1:27" ht="14.25" customHeight="1">
       <c r="A223" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B223" s="4"/>
+      <c r="B223" s="4">
+        <v>2019</v>
+      </c>
       <c r="C223" s="4" t="s">
         <v>260</v>
       </c>
@@ -11386,11 +11448,13 @@
       <c r="Z223" s="7"/>
       <c r="AA223" s="7"/>
     </row>
-    <row r="224" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="224" spans="1:27" ht="14.25" customHeight="1">
       <c r="A224" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B224" s="4"/>
+      <c r="B224" s="4">
+        <v>2019</v>
+      </c>
       <c r="C224" s="4" t="s">
         <v>260</v>
       </c>
@@ -11413,11 +11477,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="225" spans="1:9" ht="14.25" customHeight="1">
       <c r="A225" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B225" s="4"/>
+      <c r="B225" s="4">
+        <v>2019</v>
+      </c>
       <c r="C225" s="4" t="s">
         <v>260</v>
       </c>
@@ -11440,11 +11506,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="226" spans="1:9" ht="14.25" customHeight="1">
       <c r="A226" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B226" s="4"/>
+      <c r="B226" s="4">
+        <v>2019</v>
+      </c>
       <c r="C226" s="4" t="s">
         <v>260</v>
       </c>
@@ -11467,11 +11535,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="227" spans="1:9" ht="14.25" customHeight="1">
       <c r="A227" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B227" s="4"/>
+      <c r="B227" s="4">
+        <v>2019</v>
+      </c>
       <c r="C227" s="4" t="s">
         <v>260</v>
       </c>
@@ -11494,11 +11564,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="228" spans="1:9" ht="14.25" customHeight="1">
       <c r="A228" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B228" s="4"/>
+      <c r="B228" s="4">
+        <v>2019</v>
+      </c>
       <c r="C228" s="4" t="s">
         <v>260</v>
       </c>
@@ -11521,11 +11593,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="229" spans="1:9" ht="14.25" customHeight="1">
       <c r="A229" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B229" s="4"/>
+      <c r="B229" s="4">
+        <v>2019</v>
+      </c>
       <c r="C229" s="4" t="s">
         <v>260</v>
       </c>
@@ -11548,11 +11622,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="230" spans="1:9" ht="14.25" customHeight="1">
       <c r="A230" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B230" s="4"/>
+      <c r="B230" s="4">
+        <v>2019</v>
+      </c>
       <c r="C230" s="4" t="s">
         <v>260</v>
       </c>
@@ -11575,11 +11651,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="231" spans="1:9" ht="14.25" customHeight="1">
       <c r="A231" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B231" s="4"/>
+      <c r="B231" s="4">
+        <v>2019</v>
+      </c>
       <c r="C231" s="4" t="s">
         <v>260</v>
       </c>
@@ -11602,11 +11680,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="232" spans="1:9" ht="14.25" customHeight="1">
       <c r="A232" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B232" s="4"/>
+      <c r="B232" s="4">
+        <v>2019</v>
+      </c>
       <c r="C232" s="4" t="s">
         <v>260</v>
       </c>
@@ -11629,11 +11709,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="233" spans="1:9" ht="14.25" customHeight="1">
       <c r="A233" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B233" s="4"/>
+      <c r="B233" s="4">
+        <v>2019</v>
+      </c>
       <c r="C233" s="4" t="s">
         <v>260</v>
       </c>
@@ -11656,11 +11738,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="234" spans="1:9" ht="14.25" customHeight="1">
       <c r="A234" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B234" s="4"/>
+      <c r="B234" s="4">
+        <v>2019</v>
+      </c>
       <c r="C234" s="4" t="s">
         <v>260</v>
       </c>
@@ -11683,11 +11767,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="235" spans="1:9" ht="14.25" customHeight="1">
       <c r="A235" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B235" s="4"/>
+      <c r="B235" s="4">
+        <v>2019</v>
+      </c>
       <c r="C235" s="4" t="s">
         <v>260</v>
       </c>
@@ -11710,11 +11796,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="236" spans="1:9" ht="14.25" customHeight="1">
       <c r="A236" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B236" s="4"/>
+      <c r="B236" s="4">
+        <v>2019</v>
+      </c>
       <c r="C236" s="4" t="s">
         <v>260</v>
       </c>
@@ -11737,11 +11825,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="237" spans="1:9" ht="14.25" customHeight="1">
       <c r="A237" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B237" s="4"/>
+      <c r="B237" s="4">
+        <v>2019</v>
+      </c>
       <c r="C237" s="4" t="s">
         <v>260</v>
       </c>
@@ -11764,11 +11854,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="238" spans="1:9" ht="14.25" customHeight="1">
       <c r="A238" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B238" s="4"/>
+      <c r="B238" s="4">
+        <v>2019</v>
+      </c>
       <c r="C238" s="4" t="s">
         <v>260</v>
       </c>
@@ -11791,11 +11883,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="239" spans="1:9" ht="14.25" customHeight="1">
       <c r="A239" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B239" s="4"/>
+      <c r="B239" s="4">
+        <v>2019</v>
+      </c>
       <c r="C239" s="4" t="s">
         <v>260</v>
       </c>
@@ -11818,11 +11912,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="240" spans="1:9" ht="14.25" customHeight="1">
       <c r="A240" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B240" s="4"/>
+      <c r="B240" s="4">
+        <v>2019</v>
+      </c>
       <c r="C240" s="4" t="s">
         <v>260</v>
       </c>
@@ -11845,11 +11941,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="241" spans="1:9" ht="14.25" customHeight="1">
       <c r="A241" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B241" s="4"/>
+      <c r="B241" s="4">
+        <v>2019</v>
+      </c>
       <c r="C241" s="4" t="s">
         <v>260</v>
       </c>
@@ -11870,11 +11968,13 @@
       </c>
       <c r="I241" s="4"/>
     </row>
-    <row r="242" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="242" spans="1:9" ht="14.25" customHeight="1">
       <c r="A242" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B242" s="4"/>
+      <c r="B242" s="4">
+        <v>2019</v>
+      </c>
       <c r="C242" s="4" t="s">
         <v>260</v>
       </c>
@@ -11895,11 +11995,13 @@
       </c>
       <c r="I242" s="4"/>
     </row>
-    <row r="243" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="243" spans="1:9" ht="14.25" customHeight="1">
       <c r="A243" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B243" s="4"/>
+      <c r="B243" s="4">
+        <v>2019</v>
+      </c>
       <c r="C243" s="4" t="s">
         <v>260</v>
       </c>
@@ -11920,11 +12022,13 @@
       </c>
       <c r="I243" s="4"/>
     </row>
-    <row r="244" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="244" spans="1:9" ht="14.25" customHeight="1">
       <c r="A244" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B244" s="4"/>
+      <c r="B244" s="4">
+        <v>2019</v>
+      </c>
       <c r="C244" s="4" t="s">
         <v>260</v>
       </c>
@@ -11945,11 +12049,13 @@
       </c>
       <c r="I244" s="4"/>
     </row>
-    <row r="245" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="245" spans="1:9" ht="14.25" customHeight="1">
       <c r="A245" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B245" s="4"/>
+      <c r="B245" s="4">
+        <v>2019</v>
+      </c>
       <c r="C245" s="4" t="s">
         <v>260</v>
       </c>
@@ -11970,11 +12076,13 @@
       </c>
       <c r="I245" s="4"/>
     </row>
-    <row r="246" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="246" spans="1:9" ht="14.25" customHeight="1">
       <c r="A246" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B246" s="4"/>
+      <c r="B246" s="4">
+        <v>2019</v>
+      </c>
       <c r="C246" s="4" t="s">
         <v>260</v>
       </c>
@@ -11995,11 +12103,13 @@
       </c>
       <c r="I246" s="4"/>
     </row>
-    <row r="247" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="247" spans="1:9" ht="14.25" customHeight="1">
       <c r="A247" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B247" s="4"/>
+      <c r="B247" s="4">
+        <v>2019</v>
+      </c>
       <c r="C247" s="4" t="s">
         <v>260</v>
       </c>
@@ -12022,11 +12132,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="248" spans="1:9" ht="14.25" customHeight="1">
       <c r="A248" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B248" s="4"/>
+      <c r="B248" s="4">
+        <v>2019</v>
+      </c>
       <c r="C248" s="4" t="s">
         <v>260</v>
       </c>
@@ -12049,11 +12161,13 @@
         <v>325</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="249" spans="1:9" ht="14.25" customHeight="1">
       <c r="A249" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B249" s="4"/>
+      <c r="B249" s="4">
+        <v>2019</v>
+      </c>
       <c r="C249" s="4" t="s">
         <v>187</v>
       </c>
@@ -12074,11 +12188,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="250" spans="1:9" ht="14.25" customHeight="1">
       <c r="A250" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B250" s="4"/>
+      <c r="B250" s="4">
+        <v>2019</v>
+      </c>
       <c r="C250" s="4" t="s">
         <v>187</v>
       </c>
@@ -12101,11 +12217,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="251" spans="1:9" ht="14.25" customHeight="1">
       <c r="A251" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B251" s="4"/>
+      <c r="B251" s="4">
+        <v>2019</v>
+      </c>
       <c r="C251" s="4" t="s">
         <v>187</v>
       </c>
@@ -12128,11 +12246,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="252" spans="1:9" ht="14.25" customHeight="1">
       <c r="A252" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B252" s="4"/>
+      <c r="B252" s="4">
+        <v>2019</v>
+      </c>
       <c r="C252" s="4" t="s">
         <v>187</v>
       </c>
@@ -12155,11 +12275,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="253" spans="1:9" ht="14.25" customHeight="1">
       <c r="A253" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B253" s="4"/>
+      <c r="B253" s="4">
+        <v>2019</v>
+      </c>
       <c r="C253" s="4" t="s">
         <v>187</v>
       </c>
@@ -12182,11 +12304,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="254" spans="1:9" ht="14.25" customHeight="1">
       <c r="A254" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B254" s="4"/>
+      <c r="B254" s="4">
+        <v>2019</v>
+      </c>
       <c r="C254" s="4" t="s">
         <v>187</v>
       </c>
@@ -12209,11 +12333,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="255" spans="1:9" ht="14.25" customHeight="1">
       <c r="A255" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B255" s="4"/>
+      <c r="B255" s="4">
+        <v>2019</v>
+      </c>
       <c r="C255" s="4" t="s">
         <v>187</v>
       </c>
@@ -12236,11 +12362,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="256" spans="1:9" ht="14.25" customHeight="1">
       <c r="A256" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B256" s="4"/>
+      <c r="B256" s="4">
+        <v>2019</v>
+      </c>
       <c r="C256" s="4" t="s">
         <v>187</v>
       </c>
@@ -12263,11 +12391,13 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="257" spans="1:9" ht="14.25" customHeight="1">
       <c r="A257" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B257" s="4"/>
+      <c r="B257" s="4">
+        <v>2019</v>
+      </c>
       <c r="C257" s="4" t="s">
         <v>187</v>
       </c>
@@ -12290,11 +12420,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="258" spans="1:9" ht="14.25" customHeight="1">
       <c r="A258" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B258" s="4"/>
+      <c r="B258" s="4">
+        <v>2019</v>
+      </c>
       <c r="C258" s="4" t="s">
         <v>187</v>
       </c>
@@ -12317,11 +12449,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="259" spans="1:9" ht="14.25" customHeight="1">
       <c r="A259" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B259" s="4"/>
+      <c r="B259" s="4">
+        <v>2019</v>
+      </c>
       <c r="C259" s="4" t="s">
         <v>187</v>
       </c>
@@ -12344,11 +12478,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="260" spans="1:9" ht="14.25" customHeight="1">
       <c r="A260" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B260" s="4"/>
+      <c r="B260" s="4">
+        <v>2019</v>
+      </c>
       <c r="C260" s="4" t="s">
         <v>187</v>
       </c>
@@ -12371,11 +12507,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="261" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="261" spans="1:9" ht="14.25" customHeight="1">
       <c r="A261" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B261" s="4"/>
+      <c r="B261" s="4">
+        <v>2019</v>
+      </c>
       <c r="C261" s="4" t="s">
         <v>187</v>
       </c>
@@ -12398,11 +12536,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="262" spans="1:9" ht="14.25" customHeight="1">
       <c r="A262" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B262" s="4"/>
+      <c r="B262" s="4">
+        <v>2019</v>
+      </c>
       <c r="C262" s="4" t="s">
         <v>187</v>
       </c>
@@ -12425,11 +12565,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="263" spans="1:9" ht="14.25" customHeight="1">
       <c r="A263" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B263" s="4"/>
+      <c r="B263" s="4">
+        <v>2019</v>
+      </c>
       <c r="C263" s="4" t="s">
         <v>187</v>
       </c>
@@ -12452,11 +12594,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="264" spans="1:9" ht="14.25" customHeight="1">
       <c r="A264" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B264" s="4"/>
+      <c r="B264" s="4">
+        <v>2019</v>
+      </c>
       <c r="C264" s="4" t="s">
         <v>187</v>
       </c>
@@ -12479,11 +12623,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="265" spans="1:9" ht="14.25" customHeight="1">
       <c r="A265" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B265" s="4"/>
+      <c r="B265" s="4">
+        <v>2019</v>
+      </c>
       <c r="C265" s="4" t="s">
         <v>187</v>
       </c>
@@ -12506,11 +12652,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="266" spans="1:9" ht="14.25" customHeight="1">
       <c r="A266" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B266" s="4"/>
+      <c r="B266" s="4">
+        <v>2019</v>
+      </c>
       <c r="C266" s="4" t="s">
         <v>187</v>
       </c>
@@ -12533,11 +12681,13 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="267" spans="1:9" ht="14.25" customHeight="1">
       <c r="A267" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B267" s="4"/>
+      <c r="B267" s="4">
+        <v>2019</v>
+      </c>
       <c r="C267" s="4" t="s">
         <v>187</v>
       </c>
@@ -12560,11 +12710,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="268" spans="1:9" ht="14.25" customHeight="1">
       <c r="A268" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B268" s="4"/>
+      <c r="B268" s="4">
+        <v>2019</v>
+      </c>
       <c r="C268" s="4" t="s">
         <v>187</v>
       </c>
@@ -12587,11 +12739,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="269" spans="1:9" ht="14.25" customHeight="1">
       <c r="A269" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B269" s="4"/>
+      <c r="B269" s="4">
+        <v>2019</v>
+      </c>
       <c r="C269" s="4" t="s">
         <v>187</v>
       </c>
@@ -12611,14 +12765,16 @@
         <v>1280</v>
       </c>
       <c r="I269" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" ht="14.25" customHeight="1">
       <c r="A270" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B270" s="4"/>
+      <c r="B270" s="4">
+        <v>2019</v>
+      </c>
       <c r="C270" s="4" t="s">
         <v>187</v>
       </c>
@@ -12638,14 +12794,16 @@
         <v>1280</v>
       </c>
       <c r="I270" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="271" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" ht="14.25" customHeight="1">
       <c r="A271" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B271" s="4"/>
+      <c r="B271" s="4">
+        <v>2019</v>
+      </c>
       <c r="C271" s="4" t="s">
         <v>187</v>
       </c>
@@ -12668,11 +12826,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="272" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="272" spans="1:9" ht="14.25" customHeight="1">
       <c r="A272" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B272" s="4"/>
+      <c r="B272" s="4">
+        <v>2019</v>
+      </c>
       <c r="C272" s="4" t="s">
         <v>187</v>
       </c>
@@ -12695,11 +12855,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="273" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="273" spans="1:27" ht="14.25" customHeight="1">
       <c r="A273" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B273" s="4"/>
+      <c r="B273" s="4">
+        <v>2019</v>
+      </c>
       <c r="C273" s="4" t="s">
         <v>187</v>
       </c>
@@ -12722,11 +12884,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="274" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="274" spans="1:27" ht="14.25" customHeight="1">
       <c r="A274" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B274" s="4"/>
+      <c r="B274" s="4">
+        <v>2019</v>
+      </c>
       <c r="C274" s="4" t="s">
         <v>187</v>
       </c>
@@ -12749,11 +12913,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="275" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="275" spans="1:27" ht="14.25" customHeight="1">
       <c r="A275" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B275" s="4"/>
+      <c r="B275" s="4">
+        <v>2019</v>
+      </c>
       <c r="C275" s="4" t="s">
         <v>187</v>
       </c>
@@ -12773,14 +12939,16 @@
         <v>1280</v>
       </c>
       <c r="I275" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="276" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="276" spans="1:27" ht="14.25" customHeight="1">
       <c r="A276" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B276" s="4"/>
+      <c r="B276" s="4">
+        <v>2019</v>
+      </c>
       <c r="C276" s="4" t="s">
         <v>187</v>
       </c>
@@ -12800,14 +12968,16 @@
         <v>1280</v>
       </c>
       <c r="I276" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="277" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="277" spans="1:27" ht="14.25" customHeight="1">
       <c r="A277" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B277" s="4"/>
+      <c r="B277" s="4">
+        <v>2019</v>
+      </c>
       <c r="C277" s="4" t="s">
         <v>187</v>
       </c>
@@ -12830,11 +13000,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="278" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="278" spans="1:27" ht="14.25" customHeight="1">
       <c r="A278" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B278" s="4"/>
+      <c r="B278" s="4">
+        <v>2019</v>
+      </c>
       <c r="C278" s="4" t="s">
         <v>187</v>
       </c>
@@ -12857,11 +13029,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="279" spans="1:27" ht="14.25" customHeight="1">
       <c r="A279" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B279" s="4"/>
+      <c r="B279" s="4">
+        <v>2019</v>
+      </c>
       <c r="C279" s="4" t="s">
         <v>187</v>
       </c>
@@ -12884,11 +13058,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="280" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="280" spans="1:27" ht="14.25" customHeight="1">
       <c r="A280" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B280" s="4"/>
+      <c r="B280" s="4">
+        <v>2019</v>
+      </c>
       <c r="C280" s="4" t="s">
         <v>187</v>
       </c>
@@ -12909,11 +13085,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="281" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="281" spans="1:27" ht="14.25" customHeight="1">
       <c r="A281" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B281" s="4"/>
+      <c r="B281" s="4">
+        <v>2019</v>
+      </c>
       <c r="C281" s="4" t="s">
         <v>187</v>
       </c>
@@ -12954,11 +13132,13 @@
       <c r="Z281" s="7"/>
       <c r="AA281" s="7"/>
     </row>
-    <row r="282" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="282" spans="1:27" ht="14.25" customHeight="1">
       <c r="A282" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B282" s="4"/>
+      <c r="B282" s="4">
+        <v>2019</v>
+      </c>
       <c r="C282" s="4" t="s">
         <v>187</v>
       </c>
@@ -12999,11 +13179,13 @@
       <c r="Z282" s="7"/>
       <c r="AA282" s="7"/>
     </row>
-    <row r="283" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="283" spans="1:27" ht="14.25" customHeight="1">
       <c r="A283" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B283" s="4"/>
+      <c r="B283" s="4">
+        <v>2019</v>
+      </c>
       <c r="C283" s="4" t="s">
         <v>187</v>
       </c>
@@ -13044,11 +13226,13 @@
       <c r="Z283" s="7"/>
       <c r="AA283" s="7"/>
     </row>
-    <row r="284" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="284" spans="1:27" ht="14.25" customHeight="1">
       <c r="A284" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B284" s="4"/>
+      <c r="B284" s="4">
+        <v>2019</v>
+      </c>
       <c r="C284" s="4" t="s">
         <v>187</v>
       </c>
@@ -13072,11 +13256,13 @@
       </c>
       <c r="K284" s="7"/>
     </row>
-    <row r="285" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="285" spans="1:27" ht="14.25" customHeight="1">
       <c r="A285" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B285" s="4"/>
+      <c r="B285" s="4">
+        <v>2019</v>
+      </c>
       <c r="C285" s="4" t="s">
         <v>187</v>
       </c>
@@ -13100,11 +13286,13 @@
       </c>
       <c r="K285" s="7"/>
     </row>
-    <row r="286" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="286" spans="1:27" ht="14.25" customHeight="1">
       <c r="A286" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B286" s="4"/>
+      <c r="B286" s="4">
+        <v>2019</v>
+      </c>
       <c r="C286" s="4" t="s">
         <v>187</v>
       </c>
@@ -13128,11 +13316,13 @@
       </c>
       <c r="K286" s="7"/>
     </row>
-    <row r="287" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="287" spans="1:27" ht="14.25" customHeight="1">
       <c r="A287" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B287" s="4"/>
+      <c r="B287" s="4">
+        <v>2019</v>
+      </c>
       <c r="C287" s="4" t="s">
         <v>187</v>
       </c>
@@ -13156,11 +13346,13 @@
       </c>
       <c r="K287" s="7"/>
     </row>
-    <row r="288" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="288" spans="1:27" ht="14.25" customHeight="1">
       <c r="A288" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B288" s="4"/>
+      <c r="B288" s="4">
+        <v>2019</v>
+      </c>
       <c r="C288" s="4" t="s">
         <v>187</v>
       </c>
@@ -13184,11 +13376,13 @@
       </c>
       <c r="K288" s="7"/>
     </row>
-    <row r="289" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="289" spans="1:11" ht="14.25" customHeight="1">
       <c r="A289" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B289" s="4"/>
+      <c r="B289" s="4">
+        <v>2019</v>
+      </c>
       <c r="C289" s="4" t="s">
         <v>187</v>
       </c>
@@ -13212,11 +13406,13 @@
       </c>
       <c r="K289" s="7"/>
     </row>
-    <row r="290" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="290" spans="1:11" ht="14.25" customHeight="1">
       <c r="A290" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B290" s="4"/>
+      <c r="B290" s="4">
+        <v>2019</v>
+      </c>
       <c r="C290" s="4" t="s">
         <v>187</v>
       </c>
@@ -13240,11 +13436,13 @@
       </c>
       <c r="K290" s="7"/>
     </row>
-    <row r="291" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="291" spans="1:11" ht="14.25" customHeight="1">
       <c r="A291" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B291" s="4"/>
+      <c r="B291" s="4">
+        <v>2019</v>
+      </c>
       <c r="C291" s="4" t="s">
         <v>187</v>
       </c>
@@ -13268,11 +13466,13 @@
       </c>
       <c r="K291" s="7"/>
     </row>
-    <row r="292" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="292" spans="1:11" ht="14.25" customHeight="1">
       <c r="A292" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B292" s="4"/>
+      <c r="B292" s="4">
+        <v>2019</v>
+      </c>
       <c r="C292" s="4" t="s">
         <v>187</v>
       </c>
@@ -13295,11 +13495,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="293" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="293" spans="1:11" ht="14.25" customHeight="1">
       <c r="A293" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B293" s="4"/>
+      <c r="B293" s="4">
+        <v>2019</v>
+      </c>
       <c r="C293" s="4" t="s">
         <v>187</v>
       </c>
@@ -13322,11 +13524,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="294" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="294" spans="1:11" ht="14.25" customHeight="1">
       <c r="A294" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B294" s="4"/>
+      <c r="B294" s="4">
+        <v>2019</v>
+      </c>
       <c r="C294" s="4" t="s">
         <v>187</v>
       </c>
@@ -13349,11 +13553,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="295" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="295" spans="1:11" ht="14.25" customHeight="1">
       <c r="A295" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B295" s="4"/>
+      <c r="B295" s="4">
+        <v>2019</v>
+      </c>
       <c r="C295" s="4" t="s">
         <v>187</v>
       </c>
@@ -13376,11 +13582,13 @@
         <v>371</v>
       </c>
     </row>
-    <row r="296" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="296" spans="1:11" ht="14.25" customHeight="1">
       <c r="A296" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B296" s="4"/>
+      <c r="B296" s="4">
+        <v>2019</v>
+      </c>
       <c r="C296" s="4" t="s">
         <v>187</v>
       </c>
@@ -13403,11 +13611,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="297" spans="1:11" ht="14.25" customHeight="1">
       <c r="A297" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B297" s="4"/>
+      <c r="B297" s="4">
+        <v>2019</v>
+      </c>
       <c r="C297" s="4" t="s">
         <v>187</v>
       </c>
@@ -13430,11 +13640,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="298" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="298" spans="1:11" ht="14.25" customHeight="1">
       <c r="A298" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B298" s="4"/>
+      <c r="B298" s="4">
+        <v>2019</v>
+      </c>
       <c r="C298" s="4" t="s">
         <v>187</v>
       </c>
@@ -13457,11 +13669,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="299" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="299" spans="1:11" ht="14.25" customHeight="1">
       <c r="A299" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B299" s="4"/>
+      <c r="B299" s="4">
+        <v>2019</v>
+      </c>
       <c r="C299" s="4" t="s">
         <v>187</v>
       </c>
@@ -13484,11 +13698,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="300" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="300" spans="1:11" ht="14.25" customHeight="1">
       <c r="A300" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B300" s="4"/>
+      <c r="B300" s="4">
+        <v>2019</v>
+      </c>
       <c r="C300" s="4" t="s">
         <v>187</v>
       </c>
@@ -13511,11 +13727,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="301" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="301" spans="1:11" ht="14.25" customHeight="1">
       <c r="A301" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B301" s="4"/>
+      <c r="B301" s="4">
+        <v>2019</v>
+      </c>
       <c r="C301" s="4" t="s">
         <v>187</v>
       </c>
@@ -13538,11 +13756,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="302" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="302" spans="1:11" ht="14.25" customHeight="1">
       <c r="A302" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B302" s="4"/>
+      <c r="B302" s="4">
+        <v>2019</v>
+      </c>
       <c r="C302" s="4" t="s">
         <v>187</v>
       </c>
@@ -13565,11 +13785,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="303" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="303" spans="1:11" ht="14.25" customHeight="1">
       <c r="A303" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B303" s="4"/>
+      <c r="B303" s="4">
+        <v>2019</v>
+      </c>
       <c r="C303" s="4" t="s">
         <v>187</v>
       </c>
@@ -13592,11 +13814,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="304" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="304" spans="1:11" ht="14.25" customHeight="1">
       <c r="A304" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B304" s="4"/>
+      <c r="B304" s="4">
+        <v>2019</v>
+      </c>
       <c r="C304" s="4" t="s">
         <v>187</v>
       </c>
@@ -13619,11 +13843,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="305" spans="1:9" ht="14.25" customHeight="1">
       <c r="A305" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B305" s="4"/>
+      <c r="B305" s="4">
+        <v>2019</v>
+      </c>
       <c r="C305" s="4" t="s">
         <v>187</v>
       </c>
@@ -13646,11 +13872,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="306" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="306" spans="1:9" ht="14.25" customHeight="1">
       <c r="A306" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B306" s="4"/>
+      <c r="B306" s="4">
+        <v>2019</v>
+      </c>
       <c r="C306" s="4" t="s">
         <v>187</v>
       </c>
@@ -13673,11 +13901,13 @@
         <v>375</v>
       </c>
     </row>
-    <row r="307" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="307" spans="1:9" ht="14.25" customHeight="1">
       <c r="A307" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B307" s="4"/>
+      <c r="B307" s="4">
+        <v>2019</v>
+      </c>
       <c r="C307" s="4" t="s">
         <v>187</v>
       </c>
@@ -13700,11 +13930,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="308" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="308" spans="1:9" ht="14.25" customHeight="1">
       <c r="A308" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B308" s="4"/>
+      <c r="B308" s="4">
+        <v>2019</v>
+      </c>
       <c r="C308" s="4" t="s">
         <v>187</v>
       </c>
@@ -13727,11 +13959,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="309" spans="1:9" ht="14.25" customHeight="1">
       <c r="A309" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B309" s="4"/>
+      <c r="B309" s="4">
+        <v>2019</v>
+      </c>
       <c r="C309" s="4" t="s">
         <v>187</v>
       </c>
@@ -13754,11 +13988,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="310" spans="1:9" ht="14.25" customHeight="1">
       <c r="A310" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B310" s="4"/>
+      <c r="B310" s="4">
+        <v>2019</v>
+      </c>
       <c r="C310" s="4" t="s">
         <v>187</v>
       </c>
@@ -13781,11 +14017,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="311" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="311" spans="1:9" ht="14.25" customHeight="1">
       <c r="A311" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B311" s="4"/>
+      <c r="B311" s="4">
+        <v>2019</v>
+      </c>
       <c r="C311" s="4" t="s">
         <v>187</v>
       </c>
@@ -13808,11 +14046,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="312" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="312" spans="1:9" ht="14.25" customHeight="1">
       <c r="A312" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B312" s="4"/>
+      <c r="B312" s="4">
+        <v>2019</v>
+      </c>
       <c r="C312" s="4" t="s">
         <v>187</v>
       </c>
@@ -13835,11 +14075,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="313" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="313" spans="1:9" ht="14.25" customHeight="1">
       <c r="A313" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B313" s="4"/>
+      <c r="B313" s="4">
+        <v>2019</v>
+      </c>
       <c r="C313" s="4" t="s">
         <v>187</v>
       </c>
@@ -13862,11 +14104,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="314" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="314" spans="1:9" ht="14.25" customHeight="1">
       <c r="A314" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B314" s="4"/>
+      <c r="B314" s="4">
+        <v>2019</v>
+      </c>
       <c r="C314" s="4" t="s">
         <v>187</v>
       </c>
@@ -13889,11 +14133,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="315" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="315" spans="1:9" ht="14.25" customHeight="1">
       <c r="A315" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B315" s="4"/>
+      <c r="B315" s="4">
+        <v>2019</v>
+      </c>
       <c r="C315" s="4" t="s">
         <v>187</v>
       </c>
@@ -13916,11 +14162,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="316" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="316" spans="1:9" ht="14.25" customHeight="1">
       <c r="A316" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B316" s="4"/>
+      <c r="B316" s="4">
+        <v>2019</v>
+      </c>
       <c r="C316" s="4" t="s">
         <v>187</v>
       </c>
@@ -13943,11 +14191,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="317" spans="1:9" ht="14.25" customHeight="1">
       <c r="A317" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B317" s="4"/>
+      <c r="B317" s="4">
+        <v>2019</v>
+      </c>
       <c r="C317" s="4" t="s">
         <v>187</v>
       </c>
@@ -13970,11 +14220,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="318" spans="1:9" ht="14.25" customHeight="1">
       <c r="A318" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B318" s="4"/>
+      <c r="B318" s="4">
+        <v>2019</v>
+      </c>
       <c r="C318" s="4" t="s">
         <v>187</v>
       </c>
@@ -13993,11 +14245,13 @@
       </c>
       <c r="I318" s="4"/>
     </row>
-    <row r="319" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="319" spans="1:9" ht="14.25" customHeight="1">
       <c r="A319" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B319" s="4"/>
+      <c r="B319" s="4">
+        <v>2019</v>
+      </c>
       <c r="C319" s="4" t="s">
         <v>187</v>
       </c>
@@ -14016,11 +14270,13 @@
       </c>
       <c r="I319" s="4"/>
     </row>
-    <row r="320" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="320" spans="1:9" ht="14.25" customHeight="1">
       <c r="A320" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B320" s="4"/>
+      <c r="B320" s="4">
+        <v>2019</v>
+      </c>
       <c r="C320" s="4" t="s">
         <v>187</v>
       </c>
@@ -14039,11 +14295,13 @@
       </c>
       <c r="I320" s="4"/>
     </row>
-    <row r="321" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="321" spans="1:9" ht="14.25" customHeight="1">
       <c r="A321" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B321" s="4"/>
+      <c r="B321" s="4">
+        <v>2019</v>
+      </c>
       <c r="C321" s="4" t="s">
         <v>187</v>
       </c>
@@ -14062,11 +14320,13 @@
       </c>
       <c r="I321" s="4"/>
     </row>
-    <row r="322" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="322" spans="1:9" ht="14.25" customHeight="1">
       <c r="A322" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B322" s="4"/>
+      <c r="B322" s="4">
+        <v>2019</v>
+      </c>
       <c r="C322" s="4" t="s">
         <v>187</v>
       </c>
@@ -14085,11 +14345,13 @@
       </c>
       <c r="I322" s="4"/>
     </row>
-    <row r="323" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="323" spans="1:9" ht="14.25" customHeight="1">
       <c r="A323" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B323" s="4"/>
+      <c r="B323" s="4">
+        <v>2019</v>
+      </c>
       <c r="C323" s="4" t="s">
         <v>187</v>
       </c>
@@ -27946,7 +28208,7 @@
       </c>
       <c r="I839" s="4"/>
     </row>
-    <row r="840" spans="1:9" ht="14.25" customHeight="1" thickTop="1">
+    <row r="840" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A840" s="12" t="s">
         <v>920</v>
       </c>
@@ -27973,7 +28235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="841" spans="1:9" ht="14.25" customHeight="1">
+    <row r="841" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A841" s="12" t="s">
         <v>920</v>
       </c>
@@ -28000,7 +28262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="842" spans="1:9" ht="14.25" customHeight="1">
+    <row r="842" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A842" s="12" t="s">
         <v>920</v>
       </c>
@@ -28027,7 +28289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="843" spans="1:9" ht="14.25" customHeight="1">
+    <row r="843" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A843" s="12" t="s">
         <v>920</v>
       </c>
@@ -28054,7 +28316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="844" spans="1:9" ht="14.25" customHeight="1">
+    <row r="844" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A844" s="12" t="s">
         <v>920</v>
       </c>
@@ -28081,7 +28343,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="845" spans="1:9" ht="14.25" customHeight="1">
+    <row r="845" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A845" s="12" t="s">
         <v>920</v>
       </c>
@@ -28108,7 +28370,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="846" spans="1:9" ht="14.25" customHeight="1">
+    <row r="846" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A846" s="12" t="s">
         <v>920</v>
       </c>
@@ -28135,7 +28397,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="847" spans="1:9" ht="14.25" customHeight="1">
+    <row r="847" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A847" s="12" t="s">
         <v>920</v>
       </c>
@@ -28162,7 +28424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="848" spans="1:9" ht="14.25" customHeight="1">
+    <row r="848" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A848" s="12" t="s">
         <v>920</v>
       </c>
@@ -28189,7 +28451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="849" spans="1:9" ht="14.25" customHeight="1">
+    <row r="849" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A849" s="12" t="s">
         <v>920</v>
       </c>
@@ -28216,7 +28478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="850" spans="1:9" ht="14.25" customHeight="1">
+    <row r="850" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A850" s="12" t="s">
         <v>920</v>
       </c>
@@ -28243,7 +28505,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="851" spans="1:9" ht="14.25" customHeight="1">
+    <row r="851" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A851" s="12" t="s">
         <v>920</v>
       </c>
@@ -28270,7 +28532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="852" spans="1:9" ht="14.25" customHeight="1">
+    <row r="852" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A852" s="12" t="s">
         <v>920</v>
       </c>
@@ -28297,7 +28559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="853" spans="1:9" ht="14.25" customHeight="1">
+    <row r="853" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A853" s="12" t="s">
         <v>920</v>
       </c>
@@ -28324,7 +28586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="854" spans="1:9" ht="14.25" customHeight="1">
+    <row r="854" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A854" s="12" t="s">
         <v>920</v>
       </c>
@@ -28351,7 +28613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="855" spans="1:9" ht="14.25" customHeight="1">
+    <row r="855" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A855" s="12" t="s">
         <v>920</v>
       </c>
@@ -28378,7 +28640,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="856" spans="1:9" ht="14.25" customHeight="1">
+    <row r="856" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A856" s="12" t="s">
         <v>920</v>
       </c>
@@ -28405,7 +28667,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="857" spans="1:9" ht="14.25" customHeight="1">
+    <row r="857" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A857" s="12" t="s">
         <v>920</v>
       </c>
@@ -28432,7 +28694,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="858" spans="1:9" ht="14.25" customHeight="1">
+    <row r="858" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A858" s="12" t="s">
         <v>920</v>
       </c>
@@ -28459,7 +28721,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="859" spans="1:9" ht="14.25" customHeight="1">
+    <row r="859" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A859" s="12" t="s">
         <v>920</v>
       </c>
@@ -28486,7 +28748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="860" spans="1:9" ht="14.25" customHeight="1">
+    <row r="860" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A860" s="12" t="s">
         <v>920</v>
       </c>
@@ -28513,7 +28775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="861" spans="1:9" ht="14.25" customHeight="1">
+    <row r="861" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A861" s="12" t="s">
         <v>920</v>
       </c>
@@ -28540,7 +28802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="862" spans="1:9" ht="14.25" customHeight="1">
+    <row r="862" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A862" s="12" t="s">
         <v>920</v>
       </c>
@@ -28567,7 +28829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="863" spans="1:9" ht="14.25" customHeight="1">
+    <row r="863" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A863" s="12" t="s">
         <v>920</v>
       </c>
@@ -28594,7 +28856,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="864" spans="1:9" ht="14.25" customHeight="1">
+    <row r="864" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A864" s="12" t="s">
         <v>920</v>
       </c>
@@ -28621,7 +28883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="865" spans="1:9" ht="14.25" customHeight="1">
+    <row r="865" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A865" s="12" t="s">
         <v>920</v>
       </c>
@@ -28648,7 +28910,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="866" spans="1:9" ht="14.25" customHeight="1">
+    <row r="866" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A866" s="12" t="s">
         <v>920</v>
       </c>
@@ -28675,7 +28937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="867" spans="1:9" ht="14.25" customHeight="1">
+    <row r="867" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A867" s="12" t="s">
         <v>920</v>
       </c>
@@ -28702,7 +28964,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="868" spans="1:9" ht="14.25" customHeight="1">
+    <row r="868" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A868" s="12" t="s">
         <v>920</v>
       </c>
@@ -28729,7 +28991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="869" spans="1:9" ht="14.25" customHeight="1">
+    <row r="869" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A869" s="12" t="s">
         <v>920</v>
       </c>
@@ -28745,7 +29007,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="870" spans="1:9" ht="14.25" customHeight="1">
+    <row r="870" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A870" s="12" t="s">
         <v>920</v>
       </c>
@@ -28759,7 +29021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="871" spans="1:9" ht="14.25" customHeight="1">
+    <row r="871" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A871" s="12" t="s">
         <v>920</v>
       </c>
@@ -28781,7 +29043,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="872" spans="1:9" ht="14.25" customHeight="1">
+    <row r="872" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A872" s="12" t="s">
         <v>920</v>
       </c>
@@ -28808,7 +29070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="873" spans="1:9" ht="14.25" customHeight="1">
+    <row r="873" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A873" s="12" t="s">
         <v>920</v>
       </c>
@@ -28835,7 +29097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="874" spans="1:9" ht="14.25" customHeight="1">
+    <row r="874" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A874" s="12" t="s">
         <v>920</v>
       </c>
@@ -28862,7 +29124,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="875" spans="1:9" ht="14.25" customHeight="1">
+    <row r="875" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A875" s="12" t="s">
         <v>920</v>
       </c>
@@ -28889,7 +29151,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="876" spans="1:9" ht="14.25" customHeight="1">
+    <row r="876" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A876" s="12" t="s">
         <v>920</v>
       </c>
@@ -28916,7 +29178,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="877" spans="1:9" ht="14.25" customHeight="1">
+    <row r="877" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A877" s="12" t="s">
         <v>920</v>
       </c>
@@ -28943,7 +29205,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="878" spans="1:9" ht="14.25" customHeight="1">
+    <row r="878" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A878" s="12" t="s">
         <v>920</v>
       </c>
@@ -28970,7 +29232,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="879" spans="1:9" ht="14.25" customHeight="1">
+    <row r="879" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A879" s="12" t="s">
         <v>920</v>
       </c>
@@ -28997,7 +29259,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="880" spans="1:9" ht="14.25" customHeight="1">
+    <row r="880" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A880" s="12" t="s">
         <v>920</v>
       </c>
@@ -29024,7 +29286,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="881" spans="1:9" ht="14.25" customHeight="1">
+    <row r="881" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A881" s="12" t="s">
         <v>920</v>
       </c>
@@ -29051,7 +29313,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="882" spans="1:9" ht="14.25" customHeight="1">
+    <row r="882" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A882" s="12" t="s">
         <v>920</v>
       </c>
@@ -29075,7 +29337,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="883" spans="1:9" ht="14.25" customHeight="1">
+    <row r="883" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A883" s="12" t="s">
         <v>920</v>
       </c>
@@ -29102,7 +29364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="884" spans="1:9" ht="14.25" customHeight="1">
+    <row r="884" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A884" s="12" t="s">
         <v>920</v>
       </c>
@@ -29129,7 +29391,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="885" spans="1:9" ht="14.25" customHeight="1">
+    <row r="885" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A885" s="12" t="s">
         <v>920</v>
       </c>
@@ -29156,7 +29418,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="886" spans="1:9" ht="14.25" customHeight="1">
+    <row r="886" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A886" s="12" t="s">
         <v>920</v>
       </c>
@@ -29183,7 +29445,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="887" spans="1:9" ht="14.25" customHeight="1">
+    <row r="887" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A887" s="12" t="s">
         <v>920</v>
       </c>
@@ -29210,7 +29472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="888" spans="1:9" ht="14.25" customHeight="1">
+    <row r="888" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A888" s="12" t="s">
         <v>920</v>
       </c>
@@ -29237,7 +29499,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="889" spans="1:9" ht="14.25" customHeight="1">
+    <row r="889" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A889" s="12" t="s">
         <v>920</v>
       </c>
@@ -29264,7 +29526,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="890" spans="1:9" ht="14.25" customHeight="1">
+    <row r="890" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A890" s="12" t="s">
         <v>920</v>
       </c>
@@ -29291,7 +29553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="891" spans="1:9" ht="14.25" customHeight="1">
+    <row r="891" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A891" s="12" t="s">
         <v>920</v>
       </c>
@@ -29315,7 +29577,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="892" spans="1:9" ht="14.25" customHeight="1">
+    <row r="892" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A892" s="12" t="s">
         <v>920</v>
       </c>
@@ -29342,7 +29604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="893" spans="1:9" ht="14.25" customHeight="1">
+    <row r="893" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A893" s="12" t="s">
         <v>920</v>
       </c>
@@ -29369,7 +29631,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="894" spans="1:9" ht="14.25" customHeight="1">
+    <row r="894" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A894" s="12" t="s">
         <v>920</v>
       </c>
@@ -29396,7 +29658,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="895" spans="1:9" ht="14.25" customHeight="1">
+    <row r="895" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A895" s="12" t="s">
         <v>920</v>
       </c>
@@ -29423,7 +29685,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="896" spans="1:9" ht="14.25" customHeight="1">
+    <row r="896" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A896" s="12" t="s">
         <v>920</v>
       </c>
@@ -29450,7 +29712,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="897" spans="1:9" ht="14.25" customHeight="1">
+    <row r="897" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A897" s="12" t="s">
         <v>920</v>
       </c>
@@ -29477,7 +29739,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="898" spans="1:9" ht="14.25" customHeight="1">
+    <row r="898" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A898" s="12" t="s">
         <v>920</v>
       </c>
@@ -29498,7 +29760,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="899" spans="1:9" ht="14.25" customHeight="1">
+    <row r="899" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A899" s="12" t="s">
         <v>920</v>
       </c>
@@ -29522,7 +29784,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="900" spans="1:9" ht="14.25" customHeight="1">
+    <row r="900" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A900" s="12" t="s">
         <v>920</v>
       </c>
@@ -29546,7 +29808,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="901" spans="1:9" ht="14.25" customHeight="1">
+    <row r="901" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A901" s="12" t="s">
         <v>920</v>
       </c>
@@ -29570,7 +29832,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="902" spans="1:9" ht="14.25" customHeight="1">
+    <row r="902" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A902" s="12" t="s">
         <v>920</v>
       </c>
@@ -29594,7 +29856,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="903" spans="1:9" ht="14.25" customHeight="1">
+    <row r="903" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A903" s="12" t="s">
         <v>920</v>
       </c>
@@ -29618,7 +29880,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="904" spans="1:9" ht="14.25" customHeight="1">
+    <row r="904" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A904" s="12" t="s">
         <v>920</v>
       </c>
@@ -29642,7 +29904,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="905" spans="1:9" ht="14.25" customHeight="1">
+    <row r="905" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A905" s="12" t="s">
         <v>920</v>
       </c>
@@ -29666,7 +29928,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="906" spans="1:9" ht="14.25" customHeight="1">
+    <row r="906" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A906" s="12" t="s">
         <v>920</v>
       </c>
@@ -29690,7 +29952,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="907" spans="1:9" ht="14.25" customHeight="1">
+    <row r="907" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A907" s="12" t="s">
         <v>920</v>
       </c>
@@ -29714,7 +29976,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="908" spans="1:9" ht="14.25" customHeight="1">
+    <row r="908" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A908" s="12" t="s">
         <v>920</v>
       </c>
@@ -29738,7 +30000,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="909" spans="1:9" ht="14.25" customHeight="1">
+    <row r="909" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A909" s="12" t="s">
         <v>920</v>
       </c>
@@ -31939,7 +32201,8 @@
   <autoFilter ref="A1:J976" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Estados Unidos"/>
+        <filter val="El Salvador"/>
+        <filter val="Guatemala"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -64232,11 +64495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
graficos todos los paises
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Guido\Trabajo\Economia\Tematicas de Investigacion\Precariedad Mundial\precariedad.mundial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6AA255-4813-47C2-9912-9DB527E4D8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD69C80-DDE0-4EF9-85A4-21EE63A39663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Ingresos!$A$1:$G$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Links!$A$1:$E$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$J$976</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$J$981</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="Ys7tD0REepvTbqod3JWRak83uzW7UZueHs+uloU0nDM="/>
     </ext>
@@ -69,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7166" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7196" uniqueCount="1370">
   <si>
     <t>Pais</t>
   </si>
@@ -5106,8 +5117,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B297" sqref="B193:B297"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H362" sqref="H362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6162,7 +6173,7 @@
       <c r="Z38" s="7"/>
       <c r="AA38" s="7"/>
     </row>
-    <row r="39" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="39" spans="1:27" ht="14.25" customHeight="1" thickTop="1">
       <c r="A39" s="4" t="s">
         <v>9</v>
       </c>
@@ -6207,7 +6218,7 @@
       <c r="Z39" s="7"/>
       <c r="AA39" s="7"/>
     </row>
-    <row r="40" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="40" spans="1:27" ht="14.25" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>9</v>
       </c>
@@ -6252,7 +6263,7 @@
       <c r="Z40" s="7"/>
       <c r="AA40" s="7"/>
     </row>
-    <row r="41" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="41" spans="1:27" ht="14.25" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>9</v>
       </c>
@@ -6297,7 +6308,7 @@
       <c r="Z41" s="7"/>
       <c r="AA41" s="7"/>
     </row>
-    <row r="42" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="42" spans="1:27" ht="14.25" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -6342,7 +6353,7 @@
       <c r="Z42" s="7"/>
       <c r="AA42" s="7"/>
     </row>
-    <row r="43" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="43" spans="1:27" ht="14.25" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>9</v>
       </c>
@@ -6586,7 +6597,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="18" hidden="1" customHeight="1">
+    <row r="52" spans="1:9" ht="18" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>9</v>
       </c>
@@ -6613,7 +6624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="18" hidden="1" customHeight="1">
+    <row r="53" spans="1:9" ht="18" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>9</v>
       </c>
@@ -6640,7 +6651,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="54" spans="1:9" ht="14.25" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>9</v>
       </c>
@@ -6667,7 +6678,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="55" spans="1:9" ht="14.25" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>9</v>
       </c>
@@ -6694,7 +6705,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="56" spans="1:9" ht="14.25" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>9</v>
       </c>
@@ -6721,7 +6732,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="57" spans="1:9" ht="14.25" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7839,7 +7850,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="99" spans="1:11" ht="14.25" customHeight="1">
       <c r="A99" s="4" t="s">
         <v>110</v>
       </c>
@@ -7866,7 +7877,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="100" spans="1:11" ht="14.25" customHeight="1">
       <c r="A100" s="4" t="s">
         <v>110</v>
       </c>
@@ -7893,7 +7904,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="101" spans="1:11" ht="14.25" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>110</v>
       </c>
@@ -7920,7 +7931,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="102" spans="1:11" ht="14.25" customHeight="1">
       <c r="A102" s="4" t="s">
         <v>110</v>
       </c>
@@ -7947,7 +7958,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="103" spans="1:11" ht="14.25" customHeight="1">
       <c r="A103" s="4" t="s">
         <v>110</v>
       </c>
@@ -8028,7 +8039,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="106" spans="1:11" ht="14.25" customHeight="1">
       <c r="A106" s="4" t="s">
         <v>110</v>
       </c>
@@ -8056,7 +8067,7 @@
       </c>
       <c r="K106" s="7"/>
     </row>
-    <row r="107" spans="1:11" ht="14.25" hidden="1" customHeight="1">
+    <row r="107" spans="1:11" ht="14.25" customHeight="1">
       <c r="A107" s="4" t="s">
         <v>110</v>
       </c>
@@ -8300,7 +8311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="116" spans="1:9" ht="14.25" customHeight="1">
       <c r="A116" s="4" t="s">
         <v>110</v>
       </c>
@@ -8327,7 +8338,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="117" spans="1:9" ht="14.25" customHeight="1">
       <c r="A117" s="4" t="s">
         <v>110</v>
       </c>
@@ -8354,7 +8365,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="118" spans="1:9" ht="14.25" customHeight="1">
       <c r="A118" s="4" t="s">
         <v>110</v>
       </c>
@@ -9805,7 +9816,7 @@
       </c>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="171" spans="1:27" ht="14.25" customHeight="1">
       <c r="A171" s="4" t="s">
         <v>186</v>
       </c>
@@ -9852,7 +9863,7 @@
       <c r="Z171" s="7"/>
       <c r="AA171" s="7"/>
     </row>
-    <row r="172" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="172" spans="1:27" ht="14.25" customHeight="1">
       <c r="A172" s="4" t="s">
         <v>186</v>
       </c>
@@ -9899,7 +9910,7 @@
       <c r="Z172" s="7"/>
       <c r="AA172" s="7"/>
     </row>
-    <row r="173" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="173" spans="1:27" ht="14.25" customHeight="1">
       <c r="A173" s="4" t="s">
         <v>186</v>
       </c>
@@ -9929,7 +9940,7 @@
       </c>
       <c r="K173" s="7"/>
     </row>
-    <row r="174" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="174" spans="1:27" ht="14.25" customHeight="1">
       <c r="A174" s="4" t="s">
         <v>186</v>
       </c>
@@ -10073,7 +10084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="179" spans="1:9" ht="14.25" customHeight="1">
       <c r="A179" s="4" t="s">
         <v>186</v>
       </c>
@@ -10102,7 +10113,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="180" spans="1:9" ht="14.25" customHeight="1">
       <c r="A180" s="4" t="s">
         <v>186</v>
       </c>
@@ -10131,7 +10142,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="181" spans="1:9" ht="14.25" customHeight="1">
       <c r="A181" s="4" t="s">
         <v>186</v>
       </c>
@@ -10160,7 +10171,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="182" spans="1:9" ht="14.25" customHeight="1">
       <c r="A182" s="4" t="s">
         <v>186</v>
       </c>
@@ -10189,7 +10200,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="183" spans="1:9" ht="14.25" customHeight="1">
       <c r="A183" s="4" t="s">
         <v>186</v>
       </c>
@@ -10218,7 +10229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="184" spans="1:9" ht="14.25" customHeight="1">
       <c r="A184" s="4" t="s">
         <v>186</v>
       </c>
@@ -10479,7 +10490,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="13.5" customHeight="1" thickTop="1">
+    <row r="193" spans="1:9" ht="13.5" hidden="1" customHeight="1" thickTop="1">
       <c r="A193" s="4" t="s">
         <v>259</v>
       </c>
@@ -10508,7 +10519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="14.25" customHeight="1">
+    <row r="194" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A194" s="4" t="s">
         <v>259</v>
       </c>
@@ -10537,7 +10548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="14.25" customHeight="1">
+    <row r="195" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A195" s="4" t="s">
         <v>259</v>
       </c>
@@ -10566,7 +10577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="14.25" customHeight="1">
+    <row r="196" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A196" s="4" t="s">
         <v>259</v>
       </c>
@@ -10595,7 +10606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="14.25" customHeight="1">
+    <row r="197" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A197" s="4" t="s">
         <v>259</v>
       </c>
@@ -10624,7 +10635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="14.25" customHeight="1">
+    <row r="198" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A198" s="4" t="s">
         <v>259</v>
       </c>
@@ -10653,7 +10664,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="14.25" customHeight="1">
+    <row r="199" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A199" s="4" t="s">
         <v>259</v>
       </c>
@@ -10682,7 +10693,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="14.25" customHeight="1">
+    <row r="200" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A200" s="4" t="s">
         <v>259</v>
       </c>
@@ -10711,7 +10722,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="14.25" customHeight="1">
+    <row r="201" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A201" s="4" t="s">
         <v>259</v>
       </c>
@@ -10740,7 +10751,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="14.25" customHeight="1">
+    <row r="202" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A202" s="4" t="s">
         <v>259</v>
       </c>
@@ -10769,7 +10780,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="14.25" customHeight="1">
+    <row r="203" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A203" s="4" t="s">
         <v>259</v>
       </c>
@@ -10798,7 +10809,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="14.25" customHeight="1">
+    <row r="204" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A204" s="4" t="s">
         <v>259</v>
       </c>
@@ -10827,7 +10838,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="14.25" customHeight="1">
+    <row r="205" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A205" s="4" t="s">
         <v>259</v>
       </c>
@@ -10856,7 +10867,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="14.25" customHeight="1">
+    <row r="206" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A206" s="4" t="s">
         <v>259</v>
       </c>
@@ -10885,7 +10896,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="14.25" customHeight="1">
+    <row r="207" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A207" s="4" t="s">
         <v>259</v>
       </c>
@@ -10914,7 +10925,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="14.25" customHeight="1">
+    <row r="208" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A208" s="4" t="s">
         <v>259</v>
       </c>
@@ -10943,7 +10954,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="209" spans="1:27" ht="14.25" customHeight="1">
+    <row r="209" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A209" s="4" t="s">
         <v>259</v>
       </c>
@@ -10972,7 +10983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:27" ht="14.25" customHeight="1">
+    <row r="210" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A210" s="4" t="s">
         <v>259</v>
       </c>
@@ -11001,7 +11012,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:27" ht="14.25" customHeight="1">
+    <row r="211" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A211" s="4" t="s">
         <v>259</v>
       </c>
@@ -11030,7 +11041,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="212" spans="1:27" ht="14.25" customHeight="1">
+    <row r="212" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A212" s="4" t="s">
         <v>259</v>
       </c>
@@ -11059,7 +11070,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:27" ht="14.25" customHeight="1">
+    <row r="213" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A213" s="4" t="s">
         <v>259</v>
       </c>
@@ -11088,7 +11099,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="214" spans="1:27" ht="14.25" customHeight="1">
+    <row r="214" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A214" s="4" t="s">
         <v>259</v>
       </c>
@@ -11117,7 +11128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:27" ht="14.25" customHeight="1">
+    <row r="215" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A215" s="4" t="s">
         <v>259</v>
       </c>
@@ -11146,7 +11157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="216" spans="1:27" ht="14.25" customHeight="1">
+    <row r="216" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A216" s="4" t="s">
         <v>259</v>
       </c>
@@ -11175,7 +11186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="217" spans="1:27" ht="14.25" customHeight="1">
+    <row r="217" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A217" s="4" t="s">
         <v>259</v>
       </c>
@@ -11204,7 +11215,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="218" spans="1:27" ht="14.25" customHeight="1">
+    <row r="218" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A218" s="4" t="s">
         <v>259</v>
       </c>
@@ -11233,7 +11244,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="219" spans="1:27" ht="14.25" customHeight="1">
+    <row r="219" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A219" s="4" t="s">
         <v>259</v>
       </c>
@@ -11506,7 +11517,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="14.25" customHeight="1">
+    <row r="226" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A226" s="4" t="s">
         <v>259</v>
       </c>
@@ -11535,7 +11546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="14.25" customHeight="1">
+    <row r="227" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A227" s="4" t="s">
         <v>259</v>
       </c>
@@ -11564,7 +11575,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="14.25" customHeight="1">
+    <row r="228" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A228" s="4" t="s">
         <v>259</v>
       </c>
@@ -11593,7 +11604,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="14.25" customHeight="1">
+    <row r="229" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A229" s="4" t="s">
         <v>259</v>
       </c>
@@ -11622,7 +11633,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="14.25" customHeight="1">
+    <row r="230" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A230" s="4" t="s">
         <v>259</v>
       </c>
@@ -11651,7 +11662,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="14.25" customHeight="1">
+    <row r="231" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A231" s="4" t="s">
         <v>259</v>
       </c>
@@ -11680,7 +11691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="14.25" customHeight="1">
+    <row r="232" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A232" s="4" t="s">
         <v>259</v>
       </c>
@@ -11709,7 +11720,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="14.25" customHeight="1">
+    <row r="233" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A233" s="4" t="s">
         <v>259</v>
       </c>
@@ -11738,7 +11749,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="14.25" customHeight="1">
+    <row r="234" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A234" s="4" t="s">
         <v>259</v>
       </c>
@@ -11767,7 +11778,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="14.25" customHeight="1">
+    <row r="235" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A235" s="4" t="s">
         <v>259</v>
       </c>
@@ -11796,7 +11807,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="14.25" customHeight="1">
+    <row r="236" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A236" s="4" t="s">
         <v>259</v>
       </c>
@@ -11825,7 +11836,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="14.25" customHeight="1">
+    <row r="237" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A237" s="4" t="s">
         <v>259</v>
       </c>
@@ -11854,7 +11865,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="14.25" customHeight="1">
+    <row r="238" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A238" s="4" t="s">
         <v>259</v>
       </c>
@@ -11941,7 +11952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="14.25" customHeight="1">
+    <row r="241" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A241" s="4" t="s">
         <v>259</v>
       </c>
@@ -11968,7 +11979,7 @@
       </c>
       <c r="I241" s="4"/>
     </row>
-    <row r="242" spans="1:9" ht="14.25" customHeight="1">
+    <row r="242" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A242" s="4" t="s">
         <v>259</v>
       </c>
@@ -11995,7 +12006,7 @@
       </c>
       <c r="I242" s="4"/>
     </row>
-    <row r="243" spans="1:9" ht="14.25" customHeight="1">
+    <row r="243" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A243" s="4" t="s">
         <v>259</v>
       </c>
@@ -12022,7 +12033,7 @@
       </c>
       <c r="I243" s="4"/>
     </row>
-    <row r="244" spans="1:9" ht="14.25" customHeight="1">
+    <row r="244" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A244" s="4" t="s">
         <v>259</v>
       </c>
@@ -12049,7 +12060,7 @@
       </c>
       <c r="I244" s="4"/>
     </row>
-    <row r="245" spans="1:9" ht="14.25" customHeight="1">
+    <row r="245" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A245" s="4" t="s">
         <v>259</v>
       </c>
@@ -12076,7 +12087,7 @@
       </c>
       <c r="I245" s="4"/>
     </row>
-    <row r="246" spans="1:9" ht="14.25" customHeight="1">
+    <row r="246" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A246" s="4" t="s">
         <v>259</v>
       </c>
@@ -12103,7 +12114,7 @@
       </c>
       <c r="I246" s="4"/>
     </row>
-    <row r="247" spans="1:9" ht="14.25" customHeight="1">
+    <row r="247" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A247" s="4" t="s">
         <v>259</v>
       </c>
@@ -12132,7 +12143,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="14.25" customHeight="1">
+    <row r="248" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A248" s="4" t="s">
         <v>259</v>
       </c>
@@ -12161,7 +12172,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="14.25" customHeight="1">
+    <row r="249" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A249" s="4" t="s">
         <v>326</v>
       </c>
@@ -12188,7 +12199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="14.25" customHeight="1">
+    <row r="250" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A250" s="4" t="s">
         <v>326</v>
       </c>
@@ -12217,7 +12228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="14.25" customHeight="1">
+    <row r="251" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A251" s="4" t="s">
         <v>326</v>
       </c>
@@ -12246,7 +12257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="14.25" customHeight="1">
+    <row r="252" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A252" s="4" t="s">
         <v>326</v>
       </c>
@@ -12275,7 +12286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="14.25" customHeight="1">
+    <row r="253" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A253" s="4" t="s">
         <v>326</v>
       </c>
@@ -12304,7 +12315,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="14.25" customHeight="1">
+    <row r="254" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A254" s="4" t="s">
         <v>326</v>
       </c>
@@ -12333,7 +12344,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="14.25" customHeight="1">
+    <row r="255" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A255" s="4" t="s">
         <v>326</v>
       </c>
@@ -12362,7 +12373,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="14.25" customHeight="1">
+    <row r="256" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A256" s="4" t="s">
         <v>326</v>
       </c>
@@ -12391,7 +12402,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="14.25" customHeight="1">
+    <row r="257" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A257" s="4" t="s">
         <v>326</v>
       </c>
@@ -12420,7 +12431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="14.25" customHeight="1">
+    <row r="258" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A258" s="4" t="s">
         <v>326</v>
       </c>
@@ -12449,7 +12460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="14.25" customHeight="1">
+    <row r="259" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A259" s="4" t="s">
         <v>326</v>
       </c>
@@ -12478,7 +12489,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="14.25" customHeight="1">
+    <row r="260" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A260" s="4" t="s">
         <v>326</v>
       </c>
@@ -12507,7 +12518,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="261" spans="1:9" ht="14.25" customHeight="1">
+    <row r="261" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A261" s="4" t="s">
         <v>326</v>
       </c>
@@ -12536,7 +12547,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="14.25" customHeight="1">
+    <row r="262" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A262" s="4" t="s">
         <v>326</v>
       </c>
@@ -12565,7 +12576,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="14.25" customHeight="1">
+    <row r="263" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A263" s="4" t="s">
         <v>326</v>
       </c>
@@ -12594,7 +12605,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="14.25" customHeight="1">
+    <row r="264" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A264" s="4" t="s">
         <v>326</v>
       </c>
@@ -12623,7 +12634,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="14.25" customHeight="1">
+    <row r="265" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A265" s="4" t="s">
         <v>326</v>
       </c>
@@ -12652,7 +12663,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="14.25" customHeight="1">
+    <row r="266" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A266" s="4" t="s">
         <v>326</v>
       </c>
@@ -12681,7 +12692,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="14.25" customHeight="1">
+    <row r="267" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A267" s="4" t="s">
         <v>326</v>
       </c>
@@ -12710,7 +12721,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="14.25" customHeight="1">
+    <row r="268" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A268" s="4" t="s">
         <v>326</v>
       </c>
@@ -12739,7 +12750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="14.25" customHeight="1">
+    <row r="269" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A269" s="4" t="s">
         <v>326</v>
       </c>
@@ -12768,7 +12779,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="14.25" customHeight="1">
+    <row r="270" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A270" s="4" t="s">
         <v>326</v>
       </c>
@@ -12797,7 +12808,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="271" spans="1:9" ht="14.25" customHeight="1">
+    <row r="271" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A271" s="4" t="s">
         <v>326</v>
       </c>
@@ -12826,7 +12837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="272" spans="1:9" ht="14.25" customHeight="1">
+    <row r="272" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A272" s="4" t="s">
         <v>326</v>
       </c>
@@ -12855,7 +12866,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="273" spans="1:27" ht="14.25" customHeight="1">
+    <row r="273" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A273" s="4" t="s">
         <v>326</v>
       </c>
@@ -12884,7 +12895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="274" spans="1:27" ht="14.25" customHeight="1">
+    <row r="274" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A274" s="4" t="s">
         <v>326</v>
       </c>
@@ -12913,7 +12924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="275" spans="1:27" ht="14.25" customHeight="1">
+    <row r="275" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A275" s="4" t="s">
         <v>326</v>
       </c>
@@ -12942,7 +12953,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="276" spans="1:27" ht="14.25" customHeight="1">
+    <row r="276" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A276" s="4" t="s">
         <v>326</v>
       </c>
@@ -12971,7 +12982,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="277" spans="1:27" ht="14.25" customHeight="1">
+    <row r="277" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A277" s="4" t="s">
         <v>326</v>
       </c>
@@ -13000,7 +13011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="278" spans="1:27" ht="14.25" customHeight="1">
+    <row r="278" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A278" s="4" t="s">
         <v>326</v>
       </c>
@@ -13029,7 +13040,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="14.25" customHeight="1">
+    <row r="279" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A279" s="4" t="s">
         <v>326</v>
       </c>
@@ -13058,7 +13069,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="280" spans="1:27" ht="14.25" customHeight="1">
+    <row r="280" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A280" s="4" t="s">
         <v>326</v>
       </c>
@@ -13466,7 +13477,7 @@
       </c>
       <c r="K291" s="7"/>
     </row>
-    <row r="292" spans="1:11" ht="14.25" customHeight="1">
+    <row r="292" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A292" s="4" t="s">
         <v>326</v>
       </c>
@@ -13495,7 +13506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="293" spans="1:11" ht="14.25" customHeight="1">
+    <row r="293" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A293" s="4" t="s">
         <v>326</v>
       </c>
@@ -13524,7 +13535,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="294" spans="1:11" ht="14.25" customHeight="1">
+    <row r="294" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A294" s="4" t="s">
         <v>326</v>
       </c>
@@ -13553,7 +13564,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="295" spans="1:11" ht="14.25" customHeight="1">
+    <row r="295" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A295" s="4" t="s">
         <v>326</v>
       </c>
@@ -13582,7 +13593,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="296" spans="1:11" ht="14.25" customHeight="1">
+    <row r="296" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A296" s="4" t="s">
         <v>326</v>
       </c>
@@ -13611,7 +13622,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="14.25" customHeight="1">
+    <row r="297" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A297" s="4" t="s">
         <v>326</v>
       </c>
@@ -13640,7 +13651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="298" spans="1:11" ht="14.25" customHeight="1">
+    <row r="298" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A298" s="4" t="s">
         <v>326</v>
       </c>
@@ -13669,7 +13680,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="299" spans="1:11" ht="14.25" customHeight="1">
+    <row r="299" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A299" s="4" t="s">
         <v>326</v>
       </c>
@@ -13698,7 +13709,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="300" spans="1:11" ht="14.25" customHeight="1">
+    <row r="300" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A300" s="4" t="s">
         <v>326</v>
       </c>
@@ -13727,7 +13738,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="301" spans="1:11" ht="14.25" customHeight="1">
+    <row r="301" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A301" s="4" t="s">
         <v>326</v>
       </c>
@@ -13756,7 +13767,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="302" spans="1:11" ht="14.25" customHeight="1">
+    <row r="302" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A302" s="4" t="s">
         <v>326</v>
       </c>
@@ -13785,7 +13796,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="303" spans="1:11" ht="14.25" customHeight="1">
+    <row r="303" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A303" s="4" t="s">
         <v>326</v>
       </c>
@@ -13814,7 +13825,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="304" spans="1:11" ht="14.25" customHeight="1">
+    <row r="304" spans="1:11" ht="14.25" hidden="1" customHeight="1">
       <c r="A304" s="4" t="s">
         <v>326</v>
       </c>
@@ -13843,7 +13854,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="14.25" customHeight="1">
+    <row r="305" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A305" s="4" t="s">
         <v>326</v>
       </c>
@@ -13872,7 +13883,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="306" spans="1:9" ht="14.25" customHeight="1">
+    <row r="306" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A306" s="4" t="s">
         <v>326</v>
       </c>
@@ -14133,7 +14144,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="315" spans="1:9" ht="14.25" customHeight="1">
+    <row r="315" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A315" s="4" t="s">
         <v>326</v>
       </c>
@@ -14162,7 +14173,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="316" spans="1:9" ht="14.25" customHeight="1">
+    <row r="316" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A316" s="4" t="s">
         <v>326</v>
       </c>
@@ -14191,7 +14202,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="14.25" customHeight="1">
+    <row r="317" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A317" s="4" t="s">
         <v>326</v>
       </c>
@@ -14220,7 +14231,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="14.25" customHeight="1">
+    <row r="318" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A318" s="4" t="s">
         <v>326</v>
       </c>
@@ -14245,7 +14256,7 @@
       </c>
       <c r="I318" s="4"/>
     </row>
-    <row r="319" spans="1:9" ht="14.25" customHeight="1">
+    <row r="319" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A319" s="4" t="s">
         <v>326</v>
       </c>
@@ -14270,7 +14281,7 @@
       </c>
       <c r="I319" s="4"/>
     </row>
-    <row r="320" spans="1:9" ht="14.25" customHeight="1">
+    <row r="320" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A320" s="4" t="s">
         <v>326</v>
       </c>
@@ -14295,7 +14306,7 @@
       </c>
       <c r="I320" s="4"/>
     </row>
-    <row r="321" spans="1:9" ht="14.25" customHeight="1">
+    <row r="321" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A321" s="4" t="s">
         <v>326</v>
       </c>
@@ -14320,7 +14331,7 @@
       </c>
       <c r="I321" s="4"/>
     </row>
-    <row r="322" spans="1:9" ht="14.25" customHeight="1">
+    <row r="322" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A322" s="4" t="s">
         <v>326</v>
       </c>
@@ -14345,7 +14356,7 @@
       </c>
       <c r="I322" s="4"/>
     </row>
-    <row r="323" spans="1:9" ht="14.25" customHeight="1">
+    <row r="323" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A323" s="4" t="s">
         <v>326</v>
       </c>
@@ -15386,7 +15397,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="362" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="362" spans="1:9" ht="14.25" customHeight="1">
       <c r="A362" s="4" t="s">
         <v>398</v>
       </c>
@@ -15413,7 +15424,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="363" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="363" spans="1:9" ht="14.25" customHeight="1">
       <c r="A363" s="4" t="s">
         <v>398</v>
       </c>
@@ -15600,7 +15611,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="370" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="370" spans="1:9" ht="14.25" customHeight="1">
       <c r="A370" s="4" t="s">
         <v>398</v>
       </c>
@@ -16658,7 +16669,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="410" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="410" spans="1:27" ht="14.25" customHeight="1">
       <c r="A410" s="4" t="s">
         <v>444</v>
       </c>
@@ -16703,7 +16714,7 @@
       <c r="Z410" s="7"/>
       <c r="AA410" s="7"/>
     </row>
-    <row r="411" spans="1:27" ht="14.25" hidden="1" customHeight="1">
+    <row r="411" spans="1:27" ht="14.25" customHeight="1">
       <c r="A411" s="4" t="s">
         <v>444</v>
       </c>
@@ -17027,7 +17038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="423" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="423" spans="1:9" ht="14.25" customHeight="1">
       <c r="A423" s="4" t="s">
         <v>444</v>
       </c>
@@ -17054,7 +17065,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="424" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="424" spans="1:9" ht="14.25" customHeight="1">
       <c r="A424" s="4" t="s">
         <v>444</v>
       </c>
@@ -17081,7 +17092,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="425" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="425" spans="1:9" ht="14.25" customHeight="1">
       <c r="A425" s="4" t="s">
         <v>444</v>
       </c>
@@ -17108,7 +17119,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="426" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="426" spans="1:9" ht="14.25" customHeight="1">
       <c r="A426" s="4" t="s">
         <v>444</v>
       </c>
@@ -18562,7 +18573,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="480" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="480" spans="1:9" ht="14.25" customHeight="1">
       <c r="A480" s="4" t="s">
         <v>505</v>
       </c>
@@ -18589,7 +18600,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="481" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="481" spans="1:10" ht="14.25" customHeight="1">
       <c r="A481" s="4" t="s">
         <v>505</v>
       </c>
@@ -18616,7 +18627,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="482" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="482" spans="1:10" ht="14.25" customHeight="1">
       <c r="A482" s="4" t="s">
         <v>505</v>
       </c>
@@ -18641,7 +18652,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="483" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="483" spans="1:10" ht="14.25" customHeight="1">
       <c r="A483" s="4" t="s">
         <v>505</v>
       </c>
@@ -18666,7 +18677,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="484" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="484" spans="1:10" ht="14.25" customHeight="1">
       <c r="A484" s="4" t="s">
         <v>505</v>
       </c>
@@ -18693,7 +18704,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="485" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="485" spans="1:10" ht="14.25" customHeight="1">
       <c r="A485" s="4" t="s">
         <v>505</v>
       </c>
@@ -18720,7 +18731,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="486" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="486" spans="1:10" ht="14.25" customHeight="1">
       <c r="A486" s="4" t="s">
         <v>505</v>
       </c>
@@ -18747,7 +18758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="487" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="487" spans="1:10" ht="14.25" customHeight="1">
       <c r="A487" s="4" t="s">
         <v>505</v>
       </c>
@@ -20243,7 +20254,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="542" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="542" spans="1:10" ht="14.25" customHeight="1">
       <c r="A542" s="4" t="s">
         <v>597</v>
       </c>
@@ -20270,7 +20281,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="543" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="543" spans="1:10" ht="14.25" customHeight="1">
       <c r="A543" s="4" t="s">
         <v>597</v>
       </c>
@@ -20297,7 +20308,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="544" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="544" spans="1:10" ht="14.25" customHeight="1">
       <c r="A544" s="4" t="s">
         <v>597</v>
       </c>
@@ -20325,7 +20336,7 @@
       </c>
       <c r="J544" s="4"/>
     </row>
-    <row r="545" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="545" spans="1:10" ht="14.25" customHeight="1">
       <c r="A545" s="4" t="s">
         <v>597</v>
       </c>
@@ -20353,7 +20364,7 @@
       </c>
       <c r="J545" s="4"/>
     </row>
-    <row r="546" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="546" spans="1:10" ht="14.25" customHeight="1">
       <c r="A546" s="4" t="s">
         <v>597</v>
       </c>
@@ -20381,7 +20392,7 @@
       </c>
       <c r="J546" s="4"/>
     </row>
-    <row r="547" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="547" spans="1:10" ht="14.25" customHeight="1">
       <c r="A547" s="4" t="s">
         <v>597</v>
       </c>
@@ -22026,7 +22037,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="609" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="609" spans="1:10" ht="14.25" customHeight="1">
       <c r="A609" s="4" t="s">
         <v>663</v>
       </c>
@@ -22051,7 +22062,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="610" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="610" spans="1:10" ht="14.25" customHeight="1">
       <c r="A610" s="4" t="s">
         <v>663</v>
       </c>
@@ -22079,7 +22090,7 @@
       </c>
       <c r="J610" s="4"/>
     </row>
-    <row r="611" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="611" spans="1:10" ht="14.25" customHeight="1">
       <c r="A611" s="4" t="s">
         <v>663</v>
       </c>
@@ -22107,7 +22118,7 @@
       </c>
       <c r="J611" s="4"/>
     </row>
-    <row r="612" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="612" spans="1:10" ht="14.25" customHeight="1">
       <c r="A612" s="4" t="s">
         <v>663</v>
       </c>
@@ -22134,7 +22145,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="613" spans="1:10" ht="14.25" hidden="1" customHeight="1">
+    <row r="613" spans="1:10" ht="14.25" customHeight="1">
       <c r="A613" s="4" t="s">
         <v>663</v>
       </c>
@@ -23283,7 +23294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="656" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="656" spans="1:9" ht="14.25" customHeight="1">
       <c r="A656" s="4" t="s">
         <v>716</v>
       </c>
@@ -23310,7 +23321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="657" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="657" spans="1:9" ht="14.25" customHeight="1">
       <c r="A657" s="4" t="s">
         <v>716</v>
       </c>
@@ -23337,7 +23348,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="658" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="658" spans="1:9" ht="14.25" customHeight="1">
       <c r="A658" s="4" t="s">
         <v>716</v>
       </c>
@@ -23364,7 +23375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="659" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="659" spans="1:9" ht="14.25" customHeight="1">
       <c r="A659" s="4" t="s">
         <v>716</v>
       </c>
@@ -23391,7 +23402,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="660" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="660" spans="1:9" ht="14.25" customHeight="1">
       <c r="A660" s="4" t="s">
         <v>716</v>
       </c>
@@ -23418,7 +23429,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="661" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="661" spans="1:9" ht="14.25" customHeight="1">
       <c r="A661" s="4" t="s">
         <v>716</v>
       </c>
@@ -23445,7 +23456,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="662" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="662" spans="1:9" ht="14.25" customHeight="1">
       <c r="A662" s="4" t="s">
         <v>716</v>
       </c>
@@ -23472,7 +23483,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="663" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="663" spans="1:9" ht="14.25" customHeight="1">
       <c r="A663" s="4" t="s">
         <v>716</v>
       </c>
@@ -23499,7 +23510,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="664" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="664" spans="1:9" ht="14.25" customHeight="1">
       <c r="A664" s="4" t="s">
         <v>716</v>
       </c>
@@ -23526,7 +23537,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="665" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="665" spans="1:9" ht="14.25" customHeight="1">
       <c r="A665" s="4" t="s">
         <v>716</v>
       </c>
@@ -23553,7 +23564,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="666" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="666" spans="1:9" ht="14.25" customHeight="1">
       <c r="A666" s="4" t="s">
         <v>716</v>
       </c>
@@ -23580,7 +23591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="667" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="667" spans="1:9" ht="14.25" customHeight="1">
       <c r="A667" s="4" t="s">
         <v>716</v>
       </c>
@@ -23607,7 +23618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="668" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="668" spans="1:9" ht="14.25" customHeight="1">
       <c r="A668" s="4" t="s">
         <v>716</v>
       </c>
@@ -23634,7 +23645,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="669" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="669" spans="1:9" ht="14.25" customHeight="1">
       <c r="A669" s="4" t="s">
         <v>716</v>
       </c>
@@ -23661,7 +23672,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="670" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="670" spans="1:9" ht="14.25" customHeight="1">
       <c r="A670" s="4" t="s">
         <v>716</v>
       </c>
@@ -23688,7 +23699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="671" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="671" spans="1:9" ht="14.25" customHeight="1">
       <c r="A671" s="4" t="s">
         <v>716</v>
       </c>
@@ -25221,7 +25232,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="728" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="728" spans="1:9" ht="15" customHeight="1">
       <c r="A728" s="4" t="s">
         <v>773</v>
       </c>
@@ -25248,7 +25259,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="729" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="729" spans="1:9" ht="15" customHeight="1">
       <c r="A729" s="4" t="s">
         <v>773</v>
       </c>
@@ -25275,7 +25286,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="730" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="730" spans="1:9" ht="15" customHeight="1">
       <c r="A730" s="4" t="s">
         <v>773</v>
       </c>
@@ -25302,7 +25313,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="731" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="731" spans="1:9" ht="15" customHeight="1">
       <c r="A731" s="4" t="s">
         <v>773</v>
       </c>
@@ -25329,7 +25340,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="732" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="732" spans="1:9" ht="15" customHeight="1">
       <c r="A732" s="4" t="s">
         <v>773</v>
       </c>
@@ -25356,7 +25367,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="733" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="733" spans="1:9" ht="15" customHeight="1">
       <c r="A733" s="4" t="s">
         <v>773</v>
       </c>
@@ -25383,7 +25394,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="734" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="734" spans="1:9" ht="15" customHeight="1">
       <c r="A734" s="4" t="s">
         <v>773</v>
       </c>
@@ -25410,7 +25421,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="735" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="735" spans="1:9" ht="15" customHeight="1">
       <c r="A735" s="4" t="s">
         <v>773</v>
       </c>
@@ -25437,7 +25448,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="736" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="736" spans="1:9" ht="15" customHeight="1">
       <c r="A736" s="4" t="s">
         <v>773</v>
       </c>
@@ -25464,7 +25475,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="737" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="737" spans="1:9" ht="15" customHeight="1">
       <c r="A737" s="4" t="s">
         <v>773</v>
       </c>
@@ -25491,7 +25502,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="738" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="738" spans="1:9" ht="15" customHeight="1">
       <c r="A738" s="4" t="s">
         <v>773</v>
       </c>
@@ -25518,7 +25529,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="739" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="739" spans="1:9" ht="14.25" customHeight="1">
       <c r="A739" s="4" t="s">
         <v>773</v>
       </c>
@@ -27200,7 +27211,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="802" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="802" spans="1:9" ht="14.25" customHeight="1">
       <c r="A802" s="4" t="s">
         <v>827</v>
       </c>
@@ -27227,7 +27238,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="803" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="803" spans="1:9" ht="14.25" customHeight="1">
       <c r="A803" s="4" t="s">
         <v>827</v>
       </c>
@@ -27254,7 +27265,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="804" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="804" spans="1:9" ht="14.25" customHeight="1">
       <c r="A804" s="4" t="s">
         <v>827</v>
       </c>
@@ -27281,7 +27292,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="805" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="805" spans="1:9" ht="14.25" customHeight="1">
       <c r="A805" s="4" t="s">
         <v>827</v>
       </c>
@@ -27308,7 +27319,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="806" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="806" spans="1:9" ht="14.25" customHeight="1">
       <c r="A806" s="4" t="s">
         <v>827</v>
       </c>
@@ -27335,7 +27346,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="807" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="807" spans="1:9" ht="14.25" customHeight="1">
       <c r="A807" s="4" t="s">
         <v>827</v>
       </c>
@@ -27362,7 +27373,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="808" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="808" spans="1:9" ht="14.25" customHeight="1">
       <c r="A808" s="4" t="s">
         <v>827</v>
       </c>
@@ -27389,7 +27400,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="809" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="809" spans="1:9" ht="14.25" customHeight="1">
       <c r="A809" s="4" t="s">
         <v>827</v>
       </c>
@@ -27416,7 +27427,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="810" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="810" spans="1:9" ht="14.25" customHeight="1">
       <c r="A810" s="4" t="s">
         <v>827</v>
       </c>
@@ -27443,7 +27454,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="811" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="811" spans="1:9" ht="14.25" customHeight="1">
       <c r="A811" s="4" t="s">
         <v>827</v>
       </c>
@@ -27470,7 +27481,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="812" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="812" spans="1:9" ht="14.25" customHeight="1">
       <c r="A812" s="4" t="s">
         <v>827</v>
       </c>
@@ -27497,7 +27508,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="813" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="813" spans="1:9" ht="14.25" customHeight="1">
       <c r="A813" s="4" t="s">
         <v>827</v>
       </c>
@@ -27524,7 +27535,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="814" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="814" spans="1:9" ht="14.25" customHeight="1">
       <c r="A814" s="4" t="s">
         <v>827</v>
       </c>
@@ -27551,7 +27562,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="815" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="815" spans="1:9" ht="14.25" customHeight="1">
       <c r="A815" s="4" t="s">
         <v>827</v>
       </c>
@@ -27578,7 +27589,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="816" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="816" spans="1:9" ht="14.25" customHeight="1">
       <c r="A816" s="4" t="s">
         <v>827</v>
       </c>
@@ -27605,7 +27616,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="817" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="817" spans="1:9" ht="14.25" customHeight="1">
       <c r="A817" s="4" t="s">
         <v>827</v>
       </c>
@@ -27632,7 +27643,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="818" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="818" spans="1:9" ht="14.25" customHeight="1">
       <c r="A818" s="4" t="s">
         <v>827</v>
       </c>
@@ -27659,7 +27670,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="819" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="819" spans="1:9" ht="14.25" customHeight="1">
       <c r="A819" s="4" t="s">
         <v>827</v>
       </c>
@@ -27686,7 +27697,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="820" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="820" spans="1:9" ht="14.25" customHeight="1">
       <c r="A820" s="4" t="s">
         <v>827</v>
       </c>
@@ -27713,7 +27724,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="821" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="821" spans="1:9" ht="14.25" customHeight="1">
       <c r="A821" s="4" t="s">
         <v>827</v>
       </c>
@@ -27740,7 +27751,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="822" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="822" spans="1:9" ht="14.25" customHeight="1">
       <c r="A822" s="4" t="s">
         <v>827</v>
       </c>
@@ -29337,7 +29348,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="883" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="883" spans="1:9" ht="14.25" customHeight="1">
       <c r="A883" s="12" t="s">
         <v>920</v>
       </c>
@@ -29364,7 +29375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="884" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="884" spans="1:9" ht="14.25" customHeight="1">
       <c r="A884" s="12" t="s">
         <v>920</v>
       </c>
@@ -29391,7 +29402,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="885" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="885" spans="1:9" ht="14.25" customHeight="1">
       <c r="A885" s="12" t="s">
         <v>920</v>
       </c>
@@ -29418,7 +29429,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="886" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="886" spans="1:9" ht="14.25" customHeight="1">
       <c r="A886" s="12" t="s">
         <v>920</v>
       </c>
@@ -29712,7 +29723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="897" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="897" spans="1:9" ht="14.25" customHeight="1">
       <c r="A897" s="12" t="s">
         <v>920</v>
       </c>
@@ -31217,7 +31228,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="953" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="953" spans="1:8" ht="14.25" customHeight="1">
       <c r="A953" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31243,7 +31254,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="954" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="954" spans="1:8" ht="14.25" customHeight="1">
       <c r="A954" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31269,7 +31280,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="955" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="955" spans="1:8" ht="14.25" customHeight="1">
       <c r="A955" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31295,7 +31306,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="956" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="956" spans="1:8" ht="14.25" customHeight="1">
       <c r="A956" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31321,7 +31332,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="957" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="957" spans="1:8" ht="14.25" customHeight="1">
       <c r="A957" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31347,7 +31358,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="958" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="958" spans="1:8" ht="14.25" customHeight="1">
       <c r="A958" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31373,7 +31384,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="959" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="959" spans="1:8" ht="14.25" customHeight="1">
       <c r="A959" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31399,7 +31410,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="960" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="960" spans="1:8" ht="14.25" customHeight="1">
       <c r="A960" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31425,7 +31436,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="961" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="961" spans="1:8" ht="14.25" customHeight="1">
       <c r="A961" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31451,7 +31462,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="962" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="962" spans="1:8" ht="14.25" customHeight="1">
       <c r="A962" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31477,7 +31488,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="963" spans="1:8" ht="14.25" hidden="1" customHeight="1">
+    <row r="963" spans="1:8" ht="14.25" customHeight="1">
       <c r="A963" s="34" t="s">
         <v>1014</v>
       </c>
@@ -31841,67 +31852,177 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="977" spans="4:6" ht="14.25" customHeight="1">
-      <c r="D977" s="5"/>
-      <c r="F977" s="5"/>
-    </row>
-    <row r="978" spans="4:6" ht="14.25" customHeight="1">
-      <c r="D978" s="5"/>
-      <c r="F978" s="5"/>
-    </row>
-    <row r="979" spans="4:6" ht="14.25" customHeight="1">
-      <c r="D979" s="5"/>
-      <c r="F979" s="5"/>
-    </row>
-    <row r="980" spans="4:6" ht="14.25" customHeight="1">
-      <c r="D980" s="5"/>
-      <c r="F980" s="5"/>
-    </row>
-    <row r="981" spans="4:6" ht="14.25" customHeight="1">
-      <c r="D981" s="5"/>
-      <c r="F981" s="5"/>
-    </row>
-    <row r="982" spans="4:6" ht="14.25" customHeight="1">
+    <row r="977" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A977" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B977" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C977" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D977" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E977" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F977" s="5">
+        <v>1</v>
+      </c>
+      <c r="G977" s="12" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H977" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="978" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A978" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B978" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C978" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D978" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E978" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F978" s="5">
+        <v>2</v>
+      </c>
+      <c r="G978" s="12" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H978" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="979" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A979" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B979" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C979" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D979" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E979" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F979" s="5">
+        <v>3</v>
+      </c>
+      <c r="G979" s="12" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H979" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="980" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A980" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B980" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C980" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D980" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E980" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F980" s="5">
+        <v>4</v>
+      </c>
+      <c r="G980" s="12" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H980" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="981" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A981" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B981" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C981" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D981" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E981" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F981" s="12">
+        <v>5</v>
+      </c>
+      <c r="G981" s="12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H981" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="982" spans="1:8" ht="14.25" customHeight="1">
       <c r="D982" s="5"/>
       <c r="F982" s="5"/>
     </row>
-    <row r="983" spans="4:6" ht="14.25" customHeight="1">
+    <row r="983" spans="1:8" ht="14.25" customHeight="1">
       <c r="D983" s="5"/>
       <c r="F983" s="5"/>
     </row>
-    <row r="984" spans="4:6" ht="14.25" customHeight="1">
+    <row r="984" spans="1:8" ht="14.25" customHeight="1">
       <c r="D984" s="5"/>
       <c r="F984" s="5"/>
     </row>
-    <row r="985" spans="4:6" ht="14.25" customHeight="1">
+    <row r="985" spans="1:8" ht="14.25" customHeight="1">
       <c r="D985" s="5"/>
       <c r="F985" s="5"/>
     </row>
-    <row r="986" spans="4:6" ht="14.25" customHeight="1">
+    <row r="986" spans="1:8" ht="14.25" customHeight="1">
       <c r="D986" s="5"/>
       <c r="F986" s="5"/>
     </row>
-    <row r="987" spans="4:6" ht="14.25" customHeight="1">
+    <row r="987" spans="1:8" ht="14.25" customHeight="1">
       <c r="D987" s="5"/>
       <c r="F987" s="5"/>
     </row>
-    <row r="988" spans="4:6" ht="14.25" customHeight="1">
+    <row r="988" spans="1:8" ht="14.25" customHeight="1">
       <c r="D988" s="5"/>
       <c r="F988" s="5"/>
     </row>
-    <row r="989" spans="4:6" ht="14.25" customHeight="1">
+    <row r="989" spans="1:8" ht="14.25" customHeight="1">
       <c r="D989" s="5"/>
       <c r="F989" s="5"/>
     </row>
-    <row r="990" spans="4:6" ht="14.25" customHeight="1">
+    <row r="990" spans="1:8" ht="14.25" customHeight="1">
       <c r="D990" s="5"/>
       <c r="F990" s="5"/>
     </row>
-    <row r="991" spans="4:6" ht="14.25" customHeight="1">
+    <row r="991" spans="1:8" ht="14.25" customHeight="1">
       <c r="D991" s="5"/>
       <c r="F991" s="5"/>
     </row>
-    <row r="992" spans="4:6" ht="14.25" customHeight="1">
+    <row r="992" spans="1:8" ht="14.25" customHeight="1">
       <c r="D992" s="5"/>
       <c r="F992" s="5"/>
     </row>
@@ -32198,11 +32319,12 @@
       <c r="F1065" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J976" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:J981" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="7">
       <filters>
-        <filter val="El Salvador"/>
-        <filter val="Guatemala"/>
+        <filter val="PRECAREG"/>
+        <filter val="PRECASEG"/>
+        <filter val="PRECATEMP"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -34731,7 +34853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>